<commit_message>
made tabs variable per kpi selected
</commit_message>
<xml_diff>
--- a/src/assets/Attributes/dashboard_data/cookpi_per_pi.xlsx
+++ b/src/assets/Attributes/dashboard_data/cookpi_per_pi.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/635b278bdf232d4a/Documents/Projects/cookkpi/dashboard/src/assets/Attributes/dashboard_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="152" documentId="8_{47E6BB2F-6528-457D-B946-AC2DD46DA1AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8CCD73E0-E306-4EE8-B7BF-A19ADDB679C6}"/>
+  <xr:revisionPtr revIDLastSave="194" documentId="8_{47E6BB2F-6528-457D-B946-AC2DD46DA1AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C0ECEE66-EF7A-4B8B-8A1F-4B3865DCA91A}"/>
   <bookViews>
-    <workbookView xWindow="44880" yWindow="14940" windowWidth="29040" windowHeight="15720" activeTab="6" xr2:uid="{C3CBD8BC-F3E4-49AF-9A7E-08CF129859BA}"/>
+    <workbookView xWindow="44880" yWindow="14940" windowWidth="29040" windowHeight="15720" xr2:uid="{C3CBD8BC-F3E4-49AF-9A7E-08CF129859BA}"/>
   </bookViews>
   <sheets>
     <sheet name="d_kpi" sheetId="8" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="621" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="617" uniqueCount="215">
   <si>
     <t>d_kpi_id</t>
   </si>
@@ -50,9 +50,6 @@
     <t>KPIName</t>
   </si>
   <si>
-    <t>dds_id</t>
-  </si>
-  <si>
     <t>dds_name</t>
   </si>
   <si>
@@ -684,6 +681,12 @@
   </si>
   <si>
     <t>grey</t>
+  </si>
+  <si>
+    <t>%_revenue_vs_tvl</t>
+  </si>
+  <si>
+    <t>RevenueTVL</t>
   </si>
 </sst>
 </file>
@@ -1039,7 +1042,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1047,10 +1050,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{811E847D-1D99-4D4E-BEB5-8ECC254EF9D7}">
-  <dimension ref="A1:X16"/>
+  <dimension ref="A1:X17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M19" sqref="M19"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="N20" sqref="N20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1084,73 +1087,73 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
         <v>15</v>
       </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>16</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>17</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>18</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>19</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>20</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>21</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>22</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>23</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>24</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>25</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>26</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>27</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>28</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>29</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>30</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>31</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>32</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>33</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>34</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>35</v>
-      </c>
-      <c r="X1" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.45">
@@ -1158,16 +1161,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" t="s">
         <v>37</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E2" t="s">
         <v>38</v>
-      </c>
-      <c r="D2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E2" t="s">
-        <v>39</v>
       </c>
       <c r="F2">
         <v>1</v>
@@ -1185,40 +1188,40 @@
         <v>1</v>
       </c>
       <c r="K2" t="s">
+        <v>39</v>
+      </c>
+      <c r="M2">
+        <v>1</v>
+      </c>
+      <c r="N2">
+        <v>1</v>
+      </c>
+      <c r="O2" t="s">
         <v>40</v>
       </c>
-      <c r="M2">
-        <v>1</v>
-      </c>
-      <c r="N2">
-        <v>1</v>
-      </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>41</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>42</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>43</v>
       </c>
-      <c r="R2" t="s">
+      <c r="T2">
+        <v>1</v>
+      </c>
+      <c r="U2" t="s">
         <v>44</v>
       </c>
-      <c r="T2">
-        <v>1</v>
-      </c>
-      <c r="U2" t="s">
+      <c r="V2" t="s">
         <v>45</v>
-      </c>
-      <c r="V2" t="s">
-        <v>46</v>
       </c>
       <c r="W2">
         <v>0</v>
       </c>
       <c r="X2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.45">
@@ -1226,16 +1229,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" t="s">
         <v>48</v>
       </c>
-      <c r="C3" t="s">
-        <v>49</v>
-      </c>
       <c r="D3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F3">
         <v>3</v>
@@ -1253,7 +1256,7 @@
         <v>2</v>
       </c>
       <c r="K3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="L3" s="1">
         <v>4.0000000000000002E-4</v>
@@ -1265,31 +1268,31 @@
         <v>1</v>
       </c>
       <c r="O3" t="s">
+        <v>40</v>
+      </c>
+      <c r="P3" t="s">
         <v>41</v>
       </c>
-      <c r="P3" t="s">
+      <c r="Q3" t="s">
         <v>42</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="R3" t="s">
         <v>43</v>
-      </c>
-      <c r="R3" t="s">
-        <v>44</v>
       </c>
       <c r="T3">
         <v>2</v>
       </c>
       <c r="U3" t="s">
+        <v>44</v>
+      </c>
+      <c r="V3" t="s">
         <v>45</v>
-      </c>
-      <c r="V3" t="s">
-        <v>46</v>
       </c>
       <c r="W3">
         <v>0</v>
       </c>
       <c r="X3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.45">
@@ -1297,16 +1300,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" t="s">
         <v>52</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E4" t="s">
         <v>53</v>
-      </c>
-      <c r="D4" t="s">
-        <v>53</v>
-      </c>
-      <c r="E4" t="s">
-        <v>54</v>
       </c>
       <c r="F4">
         <v>3</v>
@@ -1324,7 +1327,7 @@
         <v>1</v>
       </c>
       <c r="K4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="M4">
         <v>3</v>
@@ -1333,31 +1336,31 @@
         <v>1</v>
       </c>
       <c r="O4" t="s">
+        <v>40</v>
+      </c>
+      <c r="P4" t="s">
         <v>41</v>
       </c>
-      <c r="P4" t="s">
+      <c r="Q4" t="s">
         <v>42</v>
       </c>
-      <c r="Q4" t="s">
-        <v>43</v>
-      </c>
       <c r="R4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="T4">
         <v>3</v>
       </c>
       <c r="U4" t="s">
+        <v>55</v>
+      </c>
+      <c r="V4" t="s">
         <v>56</v>
-      </c>
-      <c r="V4" t="s">
-        <v>57</v>
       </c>
       <c r="W4">
         <v>0</v>
       </c>
       <c r="X4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.45">
@@ -1365,16 +1368,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C5" t="s">
         <v>58</v>
       </c>
-      <c r="C5" t="s">
-        <v>59</v>
-      </c>
       <c r="D5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F5">
         <v>4</v>
@@ -1392,40 +1395,40 @@
         <v>1</v>
       </c>
       <c r="K5" t="s">
+        <v>39</v>
+      </c>
+      <c r="M5">
+        <v>1</v>
+      </c>
+      <c r="N5">
+        <v>1</v>
+      </c>
+      <c r="O5" t="s">
         <v>40</v>
       </c>
-      <c r="M5">
-        <v>1</v>
-      </c>
-      <c r="N5">
-        <v>1</v>
-      </c>
-      <c r="O5" t="s">
+      <c r="P5" t="s">
         <v>41</v>
       </c>
-      <c r="P5" t="s">
+      <c r="Q5" t="s">
         <v>42</v>
       </c>
-      <c r="Q5" t="s">
-        <v>43</v>
-      </c>
       <c r="R5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="T5">
         <v>4</v>
       </c>
       <c r="U5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="V5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="W5">
         <v>0</v>
       </c>
       <c r="X5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.45">
@@ -1433,16 +1436,16 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C6" t="s">
         <v>62</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>63</v>
       </c>
-      <c r="D6" t="s">
-        <v>64</v>
-      </c>
       <c r="E6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F6">
         <v>5</v>
@@ -1460,40 +1463,40 @@
         <v>1</v>
       </c>
       <c r="K6" t="s">
+        <v>64</v>
+      </c>
+      <c r="M6">
+        <v>1</v>
+      </c>
+      <c r="N6">
+        <v>1</v>
+      </c>
+      <c r="O6" t="s">
+        <v>40</v>
+      </c>
+      <c r="P6" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>42</v>
+      </c>
+      <c r="R6" t="s">
         <v>65</v>
-      </c>
-      <c r="M6">
-        <v>1</v>
-      </c>
-      <c r="N6">
-        <v>1</v>
-      </c>
-      <c r="O6" t="s">
-        <v>41</v>
-      </c>
-      <c r="P6" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>43</v>
-      </c>
-      <c r="R6" t="s">
-        <v>66</v>
       </c>
       <c r="T6">
         <v>5</v>
       </c>
       <c r="U6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="V6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="W6">
         <v>0</v>
       </c>
       <c r="X6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.45">
@@ -1501,16 +1504,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>67</v>
+      </c>
+      <c r="C7" t="s">
         <v>68</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>69</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>70</v>
-      </c>
-      <c r="E7" t="s">
-        <v>71</v>
       </c>
       <c r="F7">
         <v>6</v>
@@ -1528,40 +1531,40 @@
         <v>1</v>
       </c>
       <c r="K7" t="s">
+        <v>39</v>
+      </c>
+      <c r="M7">
+        <v>1</v>
+      </c>
+      <c r="N7">
+        <v>1</v>
+      </c>
+      <c r="O7" t="s">
         <v>40</v>
       </c>
-      <c r="M7">
-        <v>1</v>
-      </c>
-      <c r="N7">
-        <v>1</v>
-      </c>
-      <c r="O7" t="s">
+      <c r="P7" t="s">
         <v>41</v>
       </c>
-      <c r="P7" t="s">
+      <c r="Q7" t="s">
         <v>42</v>
       </c>
-      <c r="Q7" t="s">
-        <v>43</v>
-      </c>
       <c r="R7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="T7">
         <v>6</v>
       </c>
       <c r="U7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="V7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="W7">
         <v>0</v>
       </c>
       <c r="X7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.45">
@@ -1569,16 +1572,16 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
+        <v>71</v>
+      </c>
+      <c r="C8" t="s">
         <v>72</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>73</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>74</v>
-      </c>
-      <c r="E8" t="s">
-        <v>75</v>
       </c>
       <c r="F8">
         <v>1</v>
@@ -1596,40 +1599,40 @@
         <v>2</v>
       </c>
       <c r="K8" t="s">
+        <v>39</v>
+      </c>
+      <c r="M8">
+        <v>1</v>
+      </c>
+      <c r="N8">
+        <v>1</v>
+      </c>
+      <c r="O8" t="s">
         <v>40</v>
       </c>
-      <c r="M8">
-        <v>1</v>
-      </c>
-      <c r="N8">
-        <v>1</v>
-      </c>
-      <c r="O8" t="s">
+      <c r="P8" t="s">
         <v>41</v>
       </c>
-      <c r="P8" t="s">
+      <c r="Q8" t="s">
         <v>42</v>
       </c>
-      <c r="Q8" t="s">
-        <v>43</v>
-      </c>
       <c r="R8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="T8">
         <v>7</v>
       </c>
       <c r="U8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="V8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="W8">
         <v>0</v>
       </c>
       <c r="X8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.45">
@@ -1637,16 +1640,16 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
+        <v>75</v>
+      </c>
+      <c r="C9" t="s">
         <v>76</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>77</v>
       </c>
-      <c r="D9" t="s">
-        <v>78</v>
-      </c>
       <c r="E9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F9">
         <v>8</v>
@@ -1664,7 +1667,7 @@
         <v>1</v>
       </c>
       <c r="K9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="M9">
         <v>3</v>
@@ -1673,31 +1676,31 @@
         <v>1</v>
       </c>
       <c r="O9" t="s">
+        <v>40</v>
+      </c>
+      <c r="P9" t="s">
         <v>41</v>
       </c>
-      <c r="P9" t="s">
+      <c r="Q9" t="s">
         <v>42</v>
       </c>
-      <c r="Q9" t="s">
-        <v>43</v>
-      </c>
       <c r="R9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="T9">
         <v>8</v>
       </c>
       <c r="U9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="V9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="W9">
         <v>0</v>
       </c>
       <c r="X9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.45">
@@ -1705,16 +1708,16 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
+        <v>78</v>
+      </c>
+      <c r="C10" t="s">
         <v>79</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>80</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>81</v>
-      </c>
-      <c r="E10" t="s">
-        <v>82</v>
       </c>
       <c r="F10">
         <v>9</v>
@@ -1732,7 +1735,7 @@
         <v>1</v>
       </c>
       <c r="K10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="M10">
         <v>3</v>
@@ -1741,31 +1744,31 @@
         <v>1</v>
       </c>
       <c r="O10" t="s">
+        <v>40</v>
+      </c>
+      <c r="P10" t="s">
         <v>41</v>
       </c>
-      <c r="P10" t="s">
+      <c r="Q10" t="s">
         <v>42</v>
       </c>
-      <c r="Q10" t="s">
-        <v>43</v>
-      </c>
       <c r="R10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="T10">
         <v>9</v>
       </c>
       <c r="U10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="V10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="W10">
         <v>0</v>
       </c>
       <c r="X10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.45">
@@ -1773,16 +1776,16 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C11" t="s">
+        <v>82</v>
+      </c>
+      <c r="D11" t="s">
         <v>83</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>84</v>
-      </c>
-      <c r="E11" t="s">
-        <v>85</v>
       </c>
       <c r="F11">
         <v>10</v>
@@ -1800,7 +1803,7 @@
         <v>1</v>
       </c>
       <c r="K11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="M11">
         <v>2</v>
@@ -1809,31 +1812,31 @@
         <v>1</v>
       </c>
       <c r="O11" t="s">
+        <v>40</v>
+      </c>
+      <c r="P11" t="s">
         <v>41</v>
       </c>
-      <c r="P11" t="s">
+      <c r="Q11" t="s">
         <v>42</v>
       </c>
-      <c r="Q11" t="s">
-        <v>43</v>
-      </c>
       <c r="R11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="T11">
         <v>10</v>
       </c>
       <c r="U11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="V11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="W11">
         <v>1</v>
       </c>
       <c r="X11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.45">
@@ -1841,16 +1844,16 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
+        <v>86</v>
+      </c>
+      <c r="C12" t="s">
         <v>87</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>88</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>89</v>
-      </c>
-      <c r="E12" t="s">
-        <v>90</v>
       </c>
       <c r="F12">
         <v>11</v>
@@ -1868,7 +1871,7 @@
         <v>1</v>
       </c>
       <c r="K12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="M12">
         <v>1</v>
@@ -1877,31 +1880,31 @@
         <v>1</v>
       </c>
       <c r="O12" t="s">
+        <v>40</v>
+      </c>
+      <c r="P12" t="s">
         <v>41</v>
       </c>
-      <c r="P12" t="s">
+      <c r="Q12" t="s">
         <v>42</v>
       </c>
-      <c r="Q12" t="s">
-        <v>43</v>
-      </c>
       <c r="R12" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="T12">
         <v>11</v>
       </c>
       <c r="U12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="V12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="W12">
         <v>1</v>
       </c>
       <c r="X12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.45">
@@ -1909,16 +1912,16 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
+        <v>91</v>
+      </c>
+      <c r="C13" t="s">
         <v>92</v>
       </c>
-      <c r="C13" t="s">
-        <v>93</v>
-      </c>
       <c r="D13" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E13" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F13">
         <v>12</v>
@@ -1936,7 +1939,7 @@
         <v>1</v>
       </c>
       <c r="K13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="M13">
         <v>1</v>
@@ -1945,31 +1948,31 @@
         <v>1</v>
       </c>
       <c r="O13" t="s">
+        <v>40</v>
+      </c>
+      <c r="P13" t="s">
         <v>41</v>
       </c>
-      <c r="P13" t="s">
+      <c r="Q13" t="s">
         <v>42</v>
       </c>
-      <c r="Q13" t="s">
-        <v>43</v>
-      </c>
       <c r="R13" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="T13">
         <v>12</v>
       </c>
       <c r="U13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="V13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="W13">
         <v>1</v>
       </c>
       <c r="X13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.45">
@@ -1977,16 +1980,16 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
+        <v>93</v>
+      </c>
+      <c r="C14" t="s">
         <v>94</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>95</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>96</v>
-      </c>
-      <c r="E14" t="s">
-        <v>97</v>
       </c>
       <c r="F14">
         <v>13</v>
@@ -2004,7 +2007,7 @@
         <v>1</v>
       </c>
       <c r="K14" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="M14">
         <v>1</v>
@@ -2013,31 +2016,31 @@
         <v>1</v>
       </c>
       <c r="O14" t="s">
+        <v>40</v>
+      </c>
+      <c r="P14" t="s">
         <v>41</v>
       </c>
-      <c r="P14" t="s">
+      <c r="Q14" t="s">
         <v>42</v>
       </c>
-      <c r="Q14" t="s">
-        <v>43</v>
-      </c>
       <c r="R14" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="T14">
         <v>13</v>
       </c>
       <c r="U14" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="V14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="W14">
         <v>1</v>
       </c>
       <c r="X14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.45">
@@ -2045,16 +2048,16 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C15" t="s">
+        <v>98</v>
+      </c>
+      <c r="D15" t="s">
         <v>99</v>
       </c>
-      <c r="D15" t="s">
-        <v>100</v>
-      </c>
       <c r="E15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F15">
         <v>12</v>
@@ -2072,7 +2075,7 @@
         <v>2</v>
       </c>
       <c r="K15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="M15">
         <v>1</v>
@@ -2081,31 +2084,31 @@
         <v>1</v>
       </c>
       <c r="O15" t="s">
+        <v>40</v>
+      </c>
+      <c r="P15" t="s">
         <v>41</v>
       </c>
-      <c r="P15" t="s">
+      <c r="Q15" t="s">
         <v>42</v>
       </c>
-      <c r="Q15" t="s">
-        <v>43</v>
-      </c>
       <c r="R15" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="T15">
         <v>14</v>
       </c>
       <c r="U15" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="V15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="W15">
         <v>1</v>
       </c>
       <c r="X15" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="16" spans="1:24" x14ac:dyDescent="0.45">
@@ -2113,16 +2116,16 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
+        <v>100</v>
+      </c>
+      <c r="C16" t="s">
         <v>101</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
         <v>102</v>
       </c>
-      <c r="D16" t="s">
-        <v>103</v>
-      </c>
       <c r="E16" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F16">
         <v>15</v>
@@ -2140,7 +2143,7 @@
         <v>1</v>
       </c>
       <c r="K16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="M16">
         <v>1</v>
@@ -2149,31 +2152,99 @@
         <v>1</v>
       </c>
       <c r="O16" t="s">
+        <v>40</v>
+      </c>
+      <c r="P16" t="s">
         <v>41</v>
       </c>
-      <c r="P16" t="s">
+      <c r="Q16" t="s">
         <v>42</v>
       </c>
-      <c r="Q16" t="s">
-        <v>43</v>
-      </c>
       <c r="R16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="T16">
         <v>15</v>
       </c>
       <c r="U16" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="V16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="W16">
         <v>1</v>
       </c>
       <c r="X16" t="s">
-        <v>47</v>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" spans="1:24" x14ac:dyDescent="0.45">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>213</v>
+      </c>
+      <c r="C17" t="s">
+        <v>214</v>
+      </c>
+      <c r="D17" t="s">
+        <v>214</v>
+      </c>
+      <c r="E17" t="s">
+        <v>89</v>
+      </c>
+      <c r="F17">
+        <v>12</v>
+      </c>
+      <c r="G17">
+        <v>10</v>
+      </c>
+      <c r="H17">
+        <v>1</v>
+      </c>
+      <c r="I17">
+        <v>1</v>
+      </c>
+      <c r="J17">
+        <v>2</v>
+      </c>
+      <c r="K17" t="s">
+        <v>49</v>
+      </c>
+      <c r="M17">
+        <v>1</v>
+      </c>
+      <c r="N17">
+        <v>1</v>
+      </c>
+      <c r="O17" t="s">
+        <v>40</v>
+      </c>
+      <c r="P17" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>42</v>
+      </c>
+      <c r="R17" t="s">
+        <v>90</v>
+      </c>
+      <c r="T17">
+        <v>16</v>
+      </c>
+      <c r="U17" t="s">
+        <v>66</v>
+      </c>
+      <c r="V17" t="s">
+        <v>56</v>
+      </c>
+      <c r="W17">
+        <v>1</v>
+      </c>
+      <c r="X17" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -2183,25 +2254,24 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9010067A-CF14-4F37-9F88-BA65B8775ED4}">
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="7.9296875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.9296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.59765625" customWidth="1"/>
-    <col min="6" max="6" width="10.46484375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.3984375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.46484375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.59765625" customWidth="1"/>
+    <col min="5" max="5" width="10.46484375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.3984375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.46484375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2212,430 +2282,313 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>139</v>
       </c>
       <c r="E1" t="s">
         <v>140</v>
       </c>
       <c r="F1" t="s">
-        <v>141</v>
-      </c>
-      <c r="G1" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2">
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>148</v>
       </c>
       <c r="D2" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="E2" t="s">
-        <v>138</v>
+        <v>4</v>
       </c>
       <c r="F2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>3</v>
       </c>
       <c r="D3" t="s">
-        <v>4</v>
+        <v>135</v>
       </c>
       <c r="E3" t="s">
-        <v>136</v>
+        <v>6</v>
       </c>
       <c r="F3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G3" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4">
-        <v>2</v>
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
       </c>
       <c r="D4" t="s">
-        <v>6</v>
+        <v>138</v>
       </c>
       <c r="E4" t="s">
-        <v>139</v>
+        <v>147</v>
       </c>
       <c r="F4" t="s">
-        <v>148</v>
-      </c>
-      <c r="G4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>87</v>
-      </c>
-      <c r="C5">
-        <v>0</v>
+        <v>86</v>
+      </c>
+      <c r="C5" t="s">
+        <v>3</v>
       </c>
       <c r="D5" t="s">
+        <v>135</v>
+      </c>
+      <c r="E5" t="s">
         <v>4</v>
       </c>
-      <c r="E5" t="s">
-        <v>136</v>
-      </c>
       <c r="F5" t="s">
-        <v>5</v>
-      </c>
-      <c r="G5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>87</v>
-      </c>
-      <c r="C6">
-        <v>1</v>
+        <v>86</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5</v>
       </c>
       <c r="D6" t="s">
+        <v>138</v>
+      </c>
+      <c r="E6" t="s">
         <v>6</v>
       </c>
-      <c r="E6" t="s">
-        <v>139</v>
-      </c>
       <c r="F6" t="s">
-        <v>7</v>
-      </c>
-      <c r="G6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>87</v>
-      </c>
-      <c r="C7">
-        <v>2</v>
+        <v>86</v>
+      </c>
+      <c r="C7" t="s">
+        <v>164</v>
       </c>
       <c r="D7" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="E7" t="s">
-        <v>163</v>
+        <v>147</v>
       </c>
       <c r="F7" t="s">
-        <v>148</v>
-      </c>
-      <c r="G7" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>92</v>
-      </c>
-      <c r="C8">
-        <v>0</v>
+        <v>91</v>
+      </c>
+      <c r="C8" t="s">
+        <v>3</v>
       </c>
       <c r="D8" t="s">
+        <v>135</v>
+      </c>
+      <c r="E8" t="s">
         <v>4</v>
       </c>
-      <c r="E8" t="s">
-        <v>136</v>
-      </c>
       <c r="F8" t="s">
-        <v>5</v>
-      </c>
-      <c r="G8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>92</v>
-      </c>
-      <c r="C9">
-        <v>1</v>
+        <v>91</v>
+      </c>
+      <c r="C9" t="s">
+        <v>5</v>
       </c>
       <c r="D9" t="s">
+        <v>138</v>
+      </c>
+      <c r="E9" t="s">
         <v>6</v>
       </c>
-      <c r="E9" t="s">
-        <v>139</v>
-      </c>
       <c r="F9" t="s">
-        <v>7</v>
-      </c>
-      <c r="G9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10">
         <v>12</v>
       </c>
       <c r="B10" t="s">
-        <v>92</v>
-      </c>
-      <c r="C10">
-        <v>2</v>
+        <v>91</v>
+      </c>
+      <c r="C10" t="s">
+        <v>164</v>
       </c>
       <c r="D10" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="E10" t="s">
-        <v>163</v>
+        <v>147</v>
       </c>
       <c r="F10" t="s">
-        <v>148</v>
-      </c>
-      <c r="G10" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11">
         <v>13</v>
       </c>
       <c r="B11" t="s">
-        <v>94</v>
-      </c>
-      <c r="C11">
-        <v>0</v>
+        <v>93</v>
+      </c>
+      <c r="C11" t="s">
+        <v>3</v>
       </c>
       <c r="D11" t="s">
+        <v>135</v>
+      </c>
+      <c r="E11" t="s">
         <v>4</v>
       </c>
-      <c r="E11" t="s">
-        <v>136</v>
-      </c>
       <c r="F11" t="s">
-        <v>5</v>
-      </c>
-      <c r="G11" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A12">
         <v>13</v>
       </c>
       <c r="B12" t="s">
-        <v>94</v>
-      </c>
-      <c r="C12">
-        <v>1</v>
+        <v>93</v>
+      </c>
+      <c r="C12" t="s">
+        <v>5</v>
       </c>
       <c r="D12" t="s">
+        <v>138</v>
+      </c>
+      <c r="E12" t="s">
         <v>6</v>
       </c>
-      <c r="E12" t="s">
-        <v>139</v>
-      </c>
       <c r="F12" t="s">
-        <v>7</v>
-      </c>
-      <c r="G12" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13">
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>94</v>
-      </c>
-      <c r="C13">
-        <v>2</v>
+        <v>93</v>
+      </c>
+      <c r="C13" t="s">
+        <v>164</v>
       </c>
       <c r="D13" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="E13" t="s">
-        <v>163</v>
+        <v>147</v>
       </c>
       <c r="F13" t="s">
-        <v>148</v>
-      </c>
-      <c r="G13" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A14">
         <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>147</v>
-      </c>
-      <c r="C14">
-        <v>0</v>
+        <v>146</v>
+      </c>
+      <c r="C14" t="s">
+        <v>3</v>
       </c>
       <c r="D14" t="s">
+        <v>135</v>
+      </c>
+      <c r="E14" t="s">
         <v>4</v>
       </c>
-      <c r="E14" t="s">
-        <v>136</v>
-      </c>
       <c r="F14" t="s">
-        <v>5</v>
-      </c>
-      <c r="G14" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>147</v>
-      </c>
-      <c r="C15">
-        <v>1</v>
+        <v>146</v>
+      </c>
+      <c r="C15" t="s">
+        <v>5</v>
       </c>
       <c r="D15" t="s">
+        <v>138</v>
+      </c>
+      <c r="E15" t="s">
         <v>6</v>
       </c>
-      <c r="E15" t="s">
-        <v>139</v>
-      </c>
       <c r="F15" t="s">
-        <v>7</v>
-      </c>
-      <c r="G15" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A16">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>147</v>
-      </c>
-      <c r="C16">
-        <v>2</v>
+        <v>100</v>
+      </c>
+      <c r="C16" t="s">
+        <v>3</v>
       </c>
       <c r="D16" t="s">
-        <v>165</v>
+        <v>135</v>
       </c>
       <c r="E16" t="s">
-        <v>163</v>
+        <v>4</v>
       </c>
       <c r="F16" t="s">
-        <v>148</v>
-      </c>
-      <c r="G16" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A17">
-        <v>15</v>
-      </c>
-      <c r="B17" t="s">
-        <v>101</v>
-      </c>
-      <c r="C17">
-        <v>0</v>
-      </c>
-      <c r="D17" t="s">
         <v>4</v>
-      </c>
-      <c r="E17" t="s">
-        <v>136</v>
-      </c>
-      <c r="F17" t="s">
-        <v>5</v>
-      </c>
-      <c r="G17" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A18">
-        <v>15</v>
-      </c>
-      <c r="B18" t="s">
-        <v>101</v>
-      </c>
-      <c r="C18">
-        <v>1</v>
-      </c>
-      <c r="D18" t="s">
-        <v>6</v>
-      </c>
-      <c r="E18" t="s">
-        <v>139</v>
-      </c>
-      <c r="F18" t="s">
-        <v>7</v>
-      </c>
-      <c r="G18" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A19">
-        <v>15</v>
-      </c>
-      <c r="B19" t="s">
-        <v>101</v>
-      </c>
-      <c r="C19">
-        <v>2</v>
-      </c>
-      <c r="D19" t="s">
-        <v>165</v>
-      </c>
-      <c r="E19" t="s">
-        <v>163</v>
-      </c>
-      <c r="F19" t="s">
-        <v>148</v>
-      </c>
-      <c r="G19" t="s">
-        <v>148</v>
       </c>
     </row>
   </sheetData>
@@ -2663,22 +2616,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C1" t="s">
         <v>142</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>143</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>144</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>145</v>
-      </c>
-      <c r="F1" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.45">
@@ -2686,19 +2639,19 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.45">
@@ -2706,19 +2659,19 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.45">
@@ -2726,19 +2679,19 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.45">
@@ -2746,19 +2699,19 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.45">
@@ -2766,19 +2719,19 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C6" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D6" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.45">
@@ -2786,19 +2739,19 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C7" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D7" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F7" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.45">
@@ -2806,19 +2759,19 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C8" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D8" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E8" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.45">
@@ -2826,19 +2779,19 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C9" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D9" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E9" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F9" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.45">
@@ -2846,19 +2799,19 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C10" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D10" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E10" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F10" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.45">
@@ -2866,19 +2819,19 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E11" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F11" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.45">
@@ -2886,19 +2839,19 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C12" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D12" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F12" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.45">
@@ -2906,19 +2859,19 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C13" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D13" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E13" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F13" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.45">
@@ -2926,19 +2879,19 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C14" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D14" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E14" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.45">
@@ -2946,19 +2899,19 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C15" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D15" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E15" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F15" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.45">
@@ -2966,19 +2919,19 @@
         <v>0</v>
       </c>
       <c r="B16" t="s">
+        <v>211</v>
+      </c>
+      <c r="C16" t="s">
+        <v>211</v>
+      </c>
+      <c r="D16" t="s">
+        <v>211</v>
+      </c>
+      <c r="E16" t="s">
+        <v>103</v>
+      </c>
+      <c r="F16" t="s">
         <v>212</v>
-      </c>
-      <c r="C16" t="s">
-        <v>212</v>
-      </c>
-      <c r="D16" t="s">
-        <v>212</v>
-      </c>
-      <c r="E16" t="s">
-        <v>104</v>
-      </c>
-      <c r="F16" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="20" spans="3:3" x14ac:dyDescent="0.45">
@@ -3009,22 +2962,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C1" t="s">
         <v>142</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>143</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>144</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>145</v>
-      </c>
-      <c r="F1" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.45">
@@ -3032,19 +2985,19 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.45">
@@ -3052,19 +3005,19 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.45">
@@ -3072,19 +3025,19 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C4" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D4" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.45">
@@ -3092,19 +3045,19 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C5" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D5" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.45">
@@ -3112,19 +3065,19 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C6" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D6" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.45">
@@ -3132,19 +3085,19 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.45">
@@ -3152,19 +3105,19 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
+        <v>110</v>
+      </c>
+      <c r="C8" t="s">
+        <v>110</v>
+      </c>
+      <c r="D8" t="s">
+        <v>110</v>
+      </c>
+      <c r="E8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8" t="s">
         <v>111</v>
-      </c>
-      <c r="C8" t="s">
-        <v>111</v>
-      </c>
-      <c r="D8" t="s">
-        <v>111</v>
-      </c>
-      <c r="E8" t="s">
-        <v>9</v>
-      </c>
-      <c r="F8" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.45">
@@ -3172,19 +3125,19 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
+        <v>112</v>
+      </c>
+      <c r="C9" t="s">
+        <v>112</v>
+      </c>
+      <c r="D9" t="s">
+        <v>112</v>
+      </c>
+      <c r="E9" t="s">
+        <v>8</v>
+      </c>
+      <c r="F9" t="s">
         <v>113</v>
-      </c>
-      <c r="C9" t="s">
-        <v>113</v>
-      </c>
-      <c r="D9" t="s">
-        <v>113</v>
-      </c>
-      <c r="E9" t="s">
-        <v>9</v>
-      </c>
-      <c r="F9" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.45">
@@ -3192,19 +3145,19 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F10" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.45">
@@ -3212,19 +3165,19 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
+        <v>115</v>
+      </c>
+      <c r="C11" t="s">
+        <v>115</v>
+      </c>
+      <c r="D11" t="s">
+        <v>115</v>
+      </c>
+      <c r="E11" t="s">
+        <v>8</v>
+      </c>
+      <c r="F11" t="s">
         <v>116</v>
-      </c>
-      <c r="C11" t="s">
-        <v>116</v>
-      </c>
-      <c r="D11" t="s">
-        <v>116</v>
-      </c>
-      <c r="E11" t="s">
-        <v>9</v>
-      </c>
-      <c r="F11" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.45">
@@ -3232,19 +3185,19 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
+        <v>117</v>
+      </c>
+      <c r="C12" t="s">
+        <v>117</v>
+      </c>
+      <c r="D12" t="s">
+        <v>117</v>
+      </c>
+      <c r="E12" t="s">
+        <v>8</v>
+      </c>
+      <c r="F12" t="s">
         <v>118</v>
-      </c>
-      <c r="C12" t="s">
-        <v>118</v>
-      </c>
-      <c r="D12" t="s">
-        <v>118</v>
-      </c>
-      <c r="E12" t="s">
-        <v>9</v>
-      </c>
-      <c r="F12" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.45">
@@ -3252,19 +3205,19 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
+        <v>119</v>
+      </c>
+      <c r="C13" t="s">
+        <v>119</v>
+      </c>
+      <c r="D13" t="s">
+        <v>119</v>
+      </c>
+      <c r="E13" t="s">
+        <v>8</v>
+      </c>
+      <c r="F13" t="s">
         <v>120</v>
-      </c>
-      <c r="C13" t="s">
-        <v>120</v>
-      </c>
-      <c r="D13" t="s">
-        <v>120</v>
-      </c>
-      <c r="E13" t="s">
-        <v>9</v>
-      </c>
-      <c r="F13" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.45">
@@ -3272,19 +3225,19 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C14" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D14" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E14" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F14" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.45">
@@ -3292,19 +3245,19 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C15" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D15" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E15" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F15" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.45">
@@ -3312,19 +3265,19 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C16" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D16" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E16" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F16" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.45">
@@ -3332,19 +3285,19 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C17" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D17" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E17" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F17" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.45">
@@ -3352,19 +3305,19 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C18" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D18" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E18" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F18" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.45">
@@ -3372,19 +3325,19 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C19" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D19" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E19" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F19" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.45">
@@ -3392,19 +3345,19 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C20" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D20" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E20" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F20" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.45">
@@ -3412,19 +3365,19 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C21" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D21" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E21" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F21" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.45">
@@ -3432,19 +3385,19 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C22" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D22" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E22" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F22" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.45">
@@ -3452,19 +3405,19 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C23" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D23" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E23" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F23" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.45">
@@ -3472,19 +3425,19 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C24" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D24" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E24" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F24" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.45">
@@ -3492,19 +3445,19 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C25" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D25" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E25" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F25" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.45">
@@ -3512,19 +3465,19 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C26" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D26" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E26" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F26" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.45">
@@ -3532,19 +3485,19 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C27" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D27" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E27" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F27" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.45">
@@ -3552,19 +3505,19 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C28" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D28" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E28" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F28" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.45">
@@ -3572,19 +3525,19 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C29" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D29" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E29" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F29" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.45">
@@ -3592,19 +3545,19 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C30" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D30" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E30" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F30" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.45">
@@ -3612,19 +3565,19 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C31" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D31" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E31" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F31" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.45">
@@ -3632,19 +3585,19 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
+        <v>204</v>
+      </c>
+      <c r="C32" t="s">
+        <v>204</v>
+      </c>
+      <c r="D32" t="s">
+        <v>204</v>
+      </c>
+      <c r="E32" t="s">
+        <v>8</v>
+      </c>
+      <c r="F32" t="s">
         <v>205</v>
-      </c>
-      <c r="C32" t="s">
-        <v>205</v>
-      </c>
-      <c r="D32" t="s">
-        <v>205</v>
-      </c>
-      <c r="E32" t="s">
-        <v>9</v>
-      </c>
-      <c r="F32" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.45">
@@ -3652,19 +3605,19 @@
         <v>0</v>
       </c>
       <c r="B33" t="s">
+        <v>211</v>
+      </c>
+      <c r="C33" t="s">
+        <v>211</v>
+      </c>
+      <c r="D33" t="s">
+        <v>211</v>
+      </c>
+      <c r="E33" t="s">
+        <v>103</v>
+      </c>
+      <c r="F33" t="s">
         <v>212</v>
-      </c>
-      <c r="C33" t="s">
-        <v>212</v>
-      </c>
-      <c r="D33" t="s">
-        <v>212</v>
-      </c>
-      <c r="E33" t="s">
-        <v>104</v>
-      </c>
-      <c r="F33" t="s">
-        <v>213</v>
       </c>
     </row>
   </sheetData>
@@ -3689,22 +3642,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C1" t="s">
         <v>142</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>143</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>144</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>145</v>
-      </c>
-      <c r="F1" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.45">
@@ -3712,19 +3665,19 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.45">
@@ -3732,19 +3685,19 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.45">
@@ -3752,19 +3705,19 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.45">
@@ -3772,19 +3725,19 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.45">
@@ -3792,19 +3745,19 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C6" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D6" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E6" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.45">
@@ -3812,19 +3765,19 @@
         <v>0</v>
       </c>
       <c r="B7" t="s">
+        <v>211</v>
+      </c>
+      <c r="C7" t="s">
+        <v>211</v>
+      </c>
+      <c r="D7" t="s">
+        <v>211</v>
+      </c>
+      <c r="E7" t="s">
+        <v>103</v>
+      </c>
+      <c r="F7" t="s">
         <v>212</v>
-      </c>
-      <c r="C7" t="s">
-        <v>212</v>
-      </c>
-      <c r="D7" t="s">
-        <v>212</v>
-      </c>
-      <c r="E7" t="s">
-        <v>104</v>
-      </c>
-      <c r="F7" t="s">
-        <v>213</v>
       </c>
     </row>
   </sheetData>
@@ -3847,22 +3800,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C1" t="s">
         <v>142</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>143</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>144</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>145</v>
-      </c>
-      <c r="F1" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.45">
@@ -3885,19 +3838,19 @@
         <v>0</v>
       </c>
       <c r="B5" t="s">
+        <v>211</v>
+      </c>
+      <c r="C5" t="s">
+        <v>211</v>
+      </c>
+      <c r="D5" t="s">
+        <v>211</v>
+      </c>
+      <c r="E5" t="s">
+        <v>103</v>
+      </c>
+      <c r="F5" t="s">
         <v>212</v>
-      </c>
-      <c r="C5" t="s">
-        <v>212</v>
-      </c>
-      <c r="D5" t="s">
-        <v>212</v>
-      </c>
-      <c r="E5" t="s">
-        <v>104</v>
-      </c>
-      <c r="F5" t="s">
-        <v>213</v>
       </c>
     </row>
   </sheetData>
@@ -3909,7 +3862,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4088C235-30A9-4FB8-A45A-F9A41BC2AB26}">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
@@ -3924,22 +3877,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C1" t="s">
         <v>142</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>143</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>144</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>145</v>
-      </c>
-      <c r="F1" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.45">
@@ -3947,19 +3900,19 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.45">
@@ -3967,19 +3920,19 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.45">
@@ -3987,19 +3940,19 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.45">
@@ -4007,19 +3960,19 @@
         <v>0</v>
       </c>
       <c r="B5" t="s">
+        <v>211</v>
+      </c>
+      <c r="C5" t="s">
+        <v>211</v>
+      </c>
+      <c r="D5" t="s">
+        <v>211</v>
+      </c>
+      <c r="E5" t="s">
+        <v>103</v>
+      </c>
+      <c r="F5" t="s">
         <v>212</v>
-      </c>
-      <c r="C5" t="s">
-        <v>212</v>
-      </c>
-      <c r="D5" t="s">
-        <v>212</v>
-      </c>
-      <c r="E5" t="s">
-        <v>104</v>
-      </c>
-      <c r="F5" t="s">
-        <v>213</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
finally fixed the actuals
</commit_message>
<xml_diff>
--- a/src/assets/Attributes/dashboard_data/cookpi_per_pi.xlsx
+++ b/src/assets/Attributes/dashboard_data/cookpi_per_pi.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/635b278bdf232d4a/Documents/Projects/cookkpi/dashboard/src/assets/Attributes/dashboard_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="194" documentId="8_{47E6BB2F-6528-457D-B946-AC2DD46DA1AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C0ECEE66-EF7A-4B8B-8A1F-4B3865DCA91A}"/>
+  <xr:revisionPtr revIDLastSave="208" documentId="8_{47E6BB2F-6528-457D-B946-AC2DD46DA1AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2E87B7BA-2860-4987-831F-C3885C7F1C74}"/>
   <bookViews>
-    <workbookView xWindow="44880" yWindow="14940" windowWidth="29040" windowHeight="15720" xr2:uid="{C3CBD8BC-F3E4-49AF-9A7E-08CF129859BA}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14476" xr2:uid="{C3CBD8BC-F3E4-49AF-9A7E-08CF129859BA}"/>
   </bookViews>
   <sheets>
     <sheet name="d_kpi" sheetId="8" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="617" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="634" uniqueCount="218">
   <si>
     <t>d_kpi_id</t>
   </si>
@@ -687,6 +687,15 @@
   </si>
   <si>
     <t>RevenueTVL</t>
+  </si>
+  <si>
+    <t>KPIType</t>
+  </si>
+  <si>
+    <t>Transaction</t>
+  </si>
+  <si>
+    <t>Snapshot</t>
   </si>
 </sst>
 </file>
@@ -1050,10 +1059,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{811E847D-1D99-4D4E-BEB5-8ECC254EF9D7}">
-  <dimension ref="A1:X17"/>
+  <dimension ref="A1:Y17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="N20" sqref="N20"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="X17" sqref="X17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1072,17 +1081,18 @@
     <col min="12" max="12" width="6.06640625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="13.3984375" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="15.3984375" bestFit="1" customWidth="1"/>
-    <col min="15" max="17" width="14.86328125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="8.59765625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="6.73046875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="7.53125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="7.9296875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="3.9296875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="6.59765625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.3984375" customWidth="1"/>
+    <col min="16" max="18" width="14.86328125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="8.59765625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="6.73046875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="7.53125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="7.9296875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="3.9296875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="6.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1126,37 +1136,40 @@
         <v>25</v>
       </c>
       <c r="O1" t="s">
+        <v>215</v>
+      </c>
+      <c r="P1" t="s">
         <v>26</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>27</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>28</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>29</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>30</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>31</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>32</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>33</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>34</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1197,34 +1210,37 @@
         <v>1</v>
       </c>
       <c r="O2" t="s">
+        <v>216</v>
+      </c>
+      <c r="P2" t="s">
         <v>40</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>41</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>42</v>
       </c>
-      <c r="R2" t="s">
+      <c r="S2" t="s">
         <v>43</v>
       </c>
-      <c r="T2">
-        <v>1</v>
-      </c>
-      <c r="U2" t="s">
+      <c r="U2">
+        <v>1</v>
+      </c>
+      <c r="V2" t="s">
         <v>44</v>
       </c>
-      <c r="V2" t="s">
+      <c r="W2" t="s">
         <v>45</v>
       </c>
-      <c r="W2">
+      <c r="X2">
         <v>0</v>
       </c>
-      <c r="X2" t="s">
+      <c r="Y2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1268,34 +1284,37 @@
         <v>1</v>
       </c>
       <c r="O3" t="s">
+        <v>216</v>
+      </c>
+      <c r="P3" t="s">
         <v>40</v>
       </c>
-      <c r="P3" t="s">
+      <c r="Q3" t="s">
         <v>41</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="R3" t="s">
         <v>42</v>
       </c>
-      <c r="R3" t="s">
+      <c r="S3" t="s">
         <v>43</v>
       </c>
-      <c r="T3">
+      <c r="U3">
         <v>2</v>
       </c>
-      <c r="U3" t="s">
+      <c r="V3" t="s">
         <v>44</v>
       </c>
-      <c r="V3" t="s">
+      <c r="W3" t="s">
         <v>45</v>
       </c>
-      <c r="W3">
+      <c r="X3">
         <v>0</v>
       </c>
-      <c r="X3" t="s">
+      <c r="Y3" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1336,34 +1355,37 @@
         <v>1</v>
       </c>
       <c r="O4" t="s">
+        <v>216</v>
+      </c>
+      <c r="P4" t="s">
         <v>40</v>
       </c>
-      <c r="P4" t="s">
+      <c r="Q4" t="s">
         <v>41</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="R4" t="s">
         <v>42</v>
       </c>
-      <c r="R4" t="s">
+      <c r="S4" t="s">
         <v>54</v>
       </c>
-      <c r="T4">
+      <c r="U4">
         <v>3</v>
       </c>
-      <c r="U4" t="s">
+      <c r="V4" t="s">
         <v>55</v>
       </c>
-      <c r="V4" t="s">
+      <c r="W4" t="s">
         <v>56</v>
       </c>
-      <c r="W4">
+      <c r="X4">
         <v>0</v>
       </c>
-      <c r="X4" t="s">
+      <c r="Y4" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1404,34 +1426,37 @@
         <v>1</v>
       </c>
       <c r="O5" t="s">
+        <v>216</v>
+      </c>
+      <c r="P5" t="s">
         <v>40</v>
       </c>
-      <c r="P5" t="s">
+      <c r="Q5" t="s">
         <v>41</v>
       </c>
-      <c r="Q5" t="s">
+      <c r="R5" t="s">
         <v>42</v>
       </c>
-      <c r="R5" t="s">
+      <c r="S5" t="s">
         <v>59</v>
       </c>
-      <c r="T5">
+      <c r="U5">
         <v>4</v>
       </c>
-      <c r="U5" t="s">
+      <c r="V5" t="s">
         <v>60</v>
       </c>
-      <c r="V5" t="s">
+      <c r="W5" t="s">
         <v>45</v>
       </c>
-      <c r="W5">
+      <c r="X5">
         <v>0</v>
       </c>
-      <c r="X5" t="s">
+      <c r="Y5" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1472,34 +1497,37 @@
         <v>1</v>
       </c>
       <c r="O6" t="s">
+        <v>216</v>
+      </c>
+      <c r="P6" t="s">
         <v>40</v>
       </c>
-      <c r="P6" t="s">
+      <c r="Q6" t="s">
         <v>41</v>
       </c>
-      <c r="Q6" t="s">
+      <c r="R6" t="s">
         <v>42</v>
       </c>
-      <c r="R6" t="s">
+      <c r="S6" t="s">
         <v>65</v>
       </c>
-      <c r="T6">
+      <c r="U6">
         <v>5</v>
       </c>
-      <c r="U6" t="s">
+      <c r="V6" t="s">
         <v>66</v>
       </c>
-      <c r="V6" t="s">
+      <c r="W6" t="s">
         <v>45</v>
       </c>
-      <c r="W6">
+      <c r="X6">
         <v>0</v>
       </c>
-      <c r="X6" t="s">
+      <c r="Y6" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1540,34 +1568,37 @@
         <v>1</v>
       </c>
       <c r="O7" t="s">
+        <v>216</v>
+      </c>
+      <c r="P7" t="s">
         <v>40</v>
       </c>
-      <c r="P7" t="s">
+      <c r="Q7" t="s">
         <v>41</v>
       </c>
-      <c r="Q7" t="s">
+      <c r="R7" t="s">
         <v>42</v>
       </c>
-      <c r="R7" t="s">
+      <c r="S7" t="s">
         <v>70</v>
       </c>
-      <c r="T7">
+      <c r="U7">
         <v>6</v>
       </c>
-      <c r="U7" t="s">
+      <c r="V7" t="s">
         <v>66</v>
       </c>
-      <c r="V7" t="s">
+      <c r="W7" t="s">
         <v>45</v>
       </c>
-      <c r="W7">
+      <c r="X7">
         <v>0</v>
       </c>
-      <c r="X7" t="s">
+      <c r="Y7" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1608,34 +1639,37 @@
         <v>1</v>
       </c>
       <c r="O8" t="s">
+        <v>216</v>
+      </c>
+      <c r="P8" t="s">
         <v>40</v>
       </c>
-      <c r="P8" t="s">
+      <c r="Q8" t="s">
         <v>41</v>
       </c>
-      <c r="Q8" t="s">
+      <c r="R8" t="s">
         <v>42</v>
       </c>
-      <c r="R8" t="s">
+      <c r="S8" t="s">
         <v>70</v>
       </c>
-      <c r="T8">
+      <c r="U8">
         <v>7</v>
       </c>
-      <c r="U8" t="s">
+      <c r="V8" t="s">
         <v>66</v>
       </c>
-      <c r="V8" t="s">
+      <c r="W8" t="s">
         <v>45</v>
       </c>
-      <c r="W8">
+      <c r="X8">
         <v>0</v>
       </c>
-      <c r="X8" t="s">
+      <c r="Y8" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1676,34 +1710,37 @@
         <v>1</v>
       </c>
       <c r="O9" t="s">
+        <v>216</v>
+      </c>
+      <c r="P9" t="s">
         <v>40</v>
       </c>
-      <c r="P9" t="s">
+      <c r="Q9" t="s">
         <v>41</v>
       </c>
-      <c r="Q9" t="s">
+      <c r="R9" t="s">
         <v>42</v>
       </c>
-      <c r="R9" t="s">
+      <c r="S9" t="s">
         <v>70</v>
       </c>
-      <c r="T9">
+      <c r="U9">
         <v>8</v>
       </c>
-      <c r="U9" t="s">
+      <c r="V9" t="s">
         <v>66</v>
       </c>
-      <c r="V9" t="s">
+      <c r="W9" t="s">
         <v>45</v>
       </c>
-      <c r="W9">
+      <c r="X9">
         <v>0</v>
       </c>
-      <c r="X9" t="s">
+      <c r="Y9" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1744,34 +1781,37 @@
         <v>1</v>
       </c>
       <c r="O10" t="s">
+        <v>216</v>
+      </c>
+      <c r="P10" t="s">
         <v>40</v>
       </c>
-      <c r="P10" t="s">
+      <c r="Q10" t="s">
         <v>41</v>
       </c>
-      <c r="Q10" t="s">
+      <c r="R10" t="s">
         <v>42</v>
       </c>
-      <c r="R10" t="s">
+      <c r="S10" t="s">
         <v>54</v>
       </c>
-      <c r="T10">
+      <c r="U10">
         <v>9</v>
       </c>
-      <c r="U10" t="s">
+      <c r="V10" t="s">
         <v>66</v>
       </c>
-      <c r="V10" t="s">
+      <c r="W10" t="s">
         <v>45</v>
       </c>
-      <c r="W10">
+      <c r="X10">
         <v>0</v>
       </c>
-      <c r="X10" t="s">
+      <c r="Y10" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1806,40 +1846,43 @@
         <v>64</v>
       </c>
       <c r="M11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N11">
         <v>1</v>
       </c>
       <c r="O11" t="s">
+        <v>217</v>
+      </c>
+      <c r="P11" t="s">
         <v>40</v>
       </c>
-      <c r="P11" t="s">
+      <c r="Q11" t="s">
         <v>41</v>
       </c>
-      <c r="Q11" t="s">
+      <c r="R11" t="s">
         <v>42</v>
       </c>
-      <c r="R11" t="s">
+      <c r="S11" t="s">
         <v>85</v>
       </c>
-      <c r="T11">
+      <c r="U11">
         <v>10</v>
       </c>
-      <c r="U11" t="s">
+      <c r="V11" t="s">
         <v>66</v>
       </c>
-      <c r="V11" t="s">
+      <c r="W11" t="s">
         <v>56</v>
       </c>
-      <c r="W11">
-        <v>1</v>
-      </c>
-      <c r="X11" t="s">
+      <c r="X11">
+        <v>1</v>
+      </c>
+      <c r="Y11" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1880,34 +1923,37 @@
         <v>1</v>
       </c>
       <c r="O12" t="s">
+        <v>216</v>
+      </c>
+      <c r="P12" t="s">
         <v>40</v>
       </c>
-      <c r="P12" t="s">
+      <c r="Q12" t="s">
         <v>41</v>
       </c>
-      <c r="Q12" t="s">
+      <c r="R12" t="s">
         <v>42</v>
       </c>
-      <c r="R12" t="s">
+      <c r="S12" t="s">
         <v>90</v>
       </c>
-      <c r="T12">
+      <c r="U12">
         <v>11</v>
       </c>
-      <c r="U12" t="s">
+      <c r="V12" t="s">
         <v>66</v>
       </c>
-      <c r="V12" t="s">
+      <c r="W12" t="s">
         <v>56</v>
       </c>
-      <c r="W12">
-        <v>1</v>
-      </c>
-      <c r="X12" t="s">
+      <c r="X12">
+        <v>1</v>
+      </c>
+      <c r="Y12" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1948,34 +1994,37 @@
         <v>1</v>
       </c>
       <c r="O13" t="s">
+        <v>216</v>
+      </c>
+      <c r="P13" t="s">
         <v>40</v>
       </c>
-      <c r="P13" t="s">
+      <c r="Q13" t="s">
         <v>41</v>
       </c>
-      <c r="Q13" t="s">
+      <c r="R13" t="s">
         <v>42</v>
       </c>
-      <c r="R13" t="s">
+      <c r="S13" t="s">
         <v>90</v>
       </c>
-      <c r="T13">
+      <c r="U13">
         <v>12</v>
       </c>
-      <c r="U13" t="s">
+      <c r="V13" t="s">
         <v>66</v>
       </c>
-      <c r="V13" t="s">
+      <c r="W13" t="s">
         <v>56</v>
       </c>
-      <c r="W13">
-        <v>1</v>
-      </c>
-      <c r="X13" t="s">
+      <c r="X13">
+        <v>1</v>
+      </c>
+      <c r="Y13" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A14">
         <v>13</v>
       </c>
@@ -2016,34 +2065,37 @@
         <v>1</v>
       </c>
       <c r="O14" t="s">
+        <v>216</v>
+      </c>
+      <c r="P14" t="s">
         <v>40</v>
       </c>
-      <c r="P14" t="s">
+      <c r="Q14" t="s">
         <v>41</v>
       </c>
-      <c r="Q14" t="s">
+      <c r="R14" t="s">
         <v>42</v>
       </c>
-      <c r="R14" t="s">
+      <c r="S14" t="s">
         <v>97</v>
       </c>
-      <c r="T14">
+      <c r="U14">
         <v>13</v>
       </c>
-      <c r="U14" t="s">
+      <c r="V14" t="s">
         <v>66</v>
       </c>
-      <c r="V14" t="s">
+      <c r="W14" t="s">
         <v>56</v>
       </c>
-      <c r="W14">
-        <v>1</v>
-      </c>
-      <c r="X14" t="s">
+      <c r="X14">
+        <v>1</v>
+      </c>
+      <c r="Y14" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A15">
         <v>14</v>
       </c>
@@ -2084,34 +2136,37 @@
         <v>1</v>
       </c>
       <c r="O15" t="s">
+        <v>216</v>
+      </c>
+      <c r="P15" t="s">
         <v>40</v>
       </c>
-      <c r="P15" t="s">
+      <c r="Q15" t="s">
         <v>41</v>
       </c>
-      <c r="Q15" t="s">
+      <c r="R15" t="s">
         <v>42</v>
       </c>
-      <c r="R15" t="s">
+      <c r="S15" t="s">
         <v>90</v>
       </c>
-      <c r="T15">
+      <c r="U15">
         <v>14</v>
       </c>
-      <c r="U15" t="s">
+      <c r="V15" t="s">
         <v>66</v>
       </c>
-      <c r="V15" t="s">
+      <c r="W15" t="s">
         <v>56</v>
       </c>
-      <c r="W15">
-        <v>1</v>
-      </c>
-      <c r="X15" t="s">
+      <c r="X15">
+        <v>1</v>
+      </c>
+      <c r="Y15" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A16">
         <v>15</v>
       </c>
@@ -2152,34 +2207,37 @@
         <v>1</v>
       </c>
       <c r="O16" t="s">
+        <v>216</v>
+      </c>
+      <c r="P16" t="s">
         <v>40</v>
       </c>
-      <c r="P16" t="s">
+      <c r="Q16" t="s">
         <v>41</v>
       </c>
-      <c r="Q16" t="s">
+      <c r="R16" t="s">
         <v>42</v>
       </c>
-      <c r="R16" t="s">
+      <c r="S16" t="s">
         <v>97</v>
       </c>
-      <c r="T16">
+      <c r="U16">
         <v>15</v>
       </c>
-      <c r="U16" t="s">
+      <c r="V16" t="s">
         <v>66</v>
       </c>
-      <c r="V16" t="s">
+      <c r="W16" t="s">
         <v>56</v>
       </c>
-      <c r="W16">
-        <v>1</v>
-      </c>
-      <c r="X16" t="s">
+      <c r="X16">
+        <v>1</v>
+      </c>
+      <c r="Y16" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A17">
         <v>16</v>
       </c>
@@ -2220,35 +2278,39 @@
         <v>1</v>
       </c>
       <c r="O17" t="s">
+        <v>216</v>
+      </c>
+      <c r="P17" t="s">
         <v>40</v>
       </c>
-      <c r="P17" t="s">
+      <c r="Q17" t="s">
         <v>41</v>
       </c>
-      <c r="Q17" t="s">
+      <c r="R17" t="s">
         <v>42</v>
       </c>
-      <c r="R17" t="s">
+      <c r="S17" t="s">
         <v>90</v>
       </c>
-      <c r="T17">
+      <c r="U17">
         <v>16</v>
       </c>
-      <c r="U17" t="s">
+      <c r="V17" t="s">
         <v>66</v>
       </c>
-      <c r="V17" t="s">
+      <c r="W17" t="s">
         <v>56</v>
       </c>
-      <c r="W17">
-        <v>1</v>
-      </c>
-      <c r="X17" t="s">
+      <c r="X17">
+        <v>0</v>
+      </c>
+      <c r="Y17" t="s">
         <v>50</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
delete unnessecary columns and add modals
</commit_message>
<xml_diff>
--- a/src/assets/Attributes/dashboard_data/cookpi_per_pi.xlsx
+++ b/src/assets/Attributes/dashboard_data/cookpi_per_pi.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/635b278bdf232d4a/Documents/Projects/cookkpi/dashboard/src/assets/Attributes/dashboard_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="301" documentId="8_{47E6BB2F-6528-457D-B946-AC2DD46DA1AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1926D98F-54B2-4070-AAC2-8B4985C7CA31}"/>
+  <xr:revisionPtr revIDLastSave="303" documentId="8_{47E6BB2F-6528-457D-B946-AC2DD46DA1AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8ABFEC91-B696-4A95-8FC7-DEC0A9150854}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14476" xr2:uid="{C3CBD8BC-F3E4-49AF-9A7E-08CF129859BA}"/>
+    <workbookView xWindow="54480" yWindow="17760" windowWidth="16875" windowHeight="10440" xr2:uid="{C3CBD8BC-F3E4-49AF-9A7E-08CF129859BA}"/>
   </bookViews>
   <sheets>
     <sheet name="d_kpi" sheetId="8" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="698" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="698" uniqueCount="227">
   <si>
     <t>d_kpi_id</t>
   </si>
@@ -720,6 +720,9 @@
   </si>
   <si>
     <t>Marketcap/Revenue</t>
+  </si>
+  <si>
+    <t>TradingVolume</t>
   </si>
 </sst>
 </file>
@@ -1086,7 +1089,7 @@
   <dimension ref="A1:Y21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="L26" sqref="L26"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2470,10 +2473,10 @@
         <v>220</v>
       </c>
       <c r="C20" t="s">
-        <v>96</v>
+        <v>226</v>
       </c>
       <c r="D20" t="s">
-        <v>96</v>
+        <v>226</v>
       </c>
       <c r="E20" t="s">
         <v>223</v>

</xml_diff>

<commit_message>
two sidebars instead of one
</commit_message>
<xml_diff>
--- a/src/assets/Attributes/dashboard_data/cookpi_per_pi.xlsx
+++ b/src/assets/Attributes/dashboard_data/cookpi_per_pi.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/635b278bdf232d4a/Documents/Projects/cookkpi/dashboard/src/assets/Attributes/dashboard_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/635b278bdf232d4a/Documents/Projects/cookpiapp/src/assets/Attributes/dashboard_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="303" documentId="8_{47E6BB2F-6528-457D-B946-AC2DD46DA1AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8ABFEC91-B696-4A95-8FC7-DEC0A9150854}"/>
+  <xr:revisionPtr revIDLastSave="304" documentId="8_{47E6BB2F-6528-457D-B946-AC2DD46DA1AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{51005E46-5FE4-4E3D-A45F-822ADB95A483}"/>
   <bookViews>
-    <workbookView xWindow="54480" yWindow="17760" windowWidth="16875" windowHeight="10440" xr2:uid="{C3CBD8BC-F3E4-49AF-9A7E-08CF129859BA}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14476" activeTab="3" xr2:uid="{C3CBD8BC-F3E4-49AF-9A7E-08CF129859BA}"/>
   </bookViews>
   <sheets>
     <sheet name="d_kpi" sheetId="8" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="698" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="698" uniqueCount="228">
   <si>
     <t>d_kpi_id</t>
   </si>
@@ -723,6 +723,9 @@
   </si>
   <si>
     <t>TradingVolume</t>
+  </si>
+  <si>
+    <t>#ff4a00</t>
   </si>
 </sst>
 </file>
@@ -783,10 +786,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1088,7 +1087,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{811E847D-1D99-4D4E-BEB5-8ECC254EF9D7}">
   <dimension ref="A1:Y21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
@@ -3377,8 +3376,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8F231CF-1F8C-4057-B510-9BE4FB409CB9}">
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A33" sqref="A33:F33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3486,7 +3485,7 @@
         <v>8</v>
       </c>
       <c r="F5" t="s">
-        <v>107</v>
+        <v>227</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.45">

</xml_diff>

<commit_message>
fixed the calculation and made cards smaller
</commit_message>
<xml_diff>
--- a/src/assets/Attributes/dashboard_data/cookpi_per_pi.xlsx
+++ b/src/assets/Attributes/dashboard_data/cookpi_per_pi.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/635b278bdf232d4a/Documents/Projects/cookpiapp/src/assets/Attributes/dashboard_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/635b278bdf232d4a/Documents/Projects/cookkpi/dashboard/src/assets/Attributes/dashboard_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="304" documentId="8_{47E6BB2F-6528-457D-B946-AC2DD46DA1AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{51005E46-5FE4-4E3D-A45F-822ADB95A483}"/>
+  <xr:revisionPtr revIDLastSave="388" documentId="8_{47E6BB2F-6528-457D-B946-AC2DD46DA1AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{11B57CAD-94DD-4C22-BA69-3C6779DA6C57}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14476" activeTab="3" xr2:uid="{C3CBD8BC-F3E4-49AF-9A7E-08CF129859BA}"/>
+    <workbookView xWindow="11168" yWindow="0" windowWidth="11415" windowHeight="14362" activeTab="3" xr2:uid="{C3CBD8BC-F3E4-49AF-9A7E-08CF129859BA}"/>
   </bookViews>
   <sheets>
     <sheet name="d_kpi" sheetId="8" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="698" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="690" uniqueCount="234">
   <si>
     <t>d_kpi_id</t>
   </si>
@@ -53,24 +53,15 @@
     <t>dds_name</t>
   </si>
   <si>
-    <t>Blockchain.blockchain</t>
-  </si>
-  <si>
     <t>d_level0_id</t>
   </si>
   <si>
-    <t>Project.project</t>
-  </si>
-  <si>
     <t>d_level1_id</t>
   </si>
   <si>
     <t>$_tvl</t>
   </si>
   <si>
-    <t>project</t>
-  </si>
-  <si>
     <t>synthetix</t>
   </si>
   <si>
@@ -122,15 +113,6 @@
     <t>AggregateDenom</t>
   </si>
   <si>
-    <t>Level0_Attribuut</t>
-  </si>
-  <si>
-    <t>Level1_Attribuut</t>
-  </si>
-  <si>
-    <t>Level2_Attribuut</t>
-  </si>
-  <si>
     <t>GroupImage</t>
   </si>
   <si>
@@ -164,15 +146,6 @@
     <t>#</t>
   </si>
   <si>
-    <t>Directie</t>
-  </si>
-  <si>
-    <t>Afdeling</t>
-  </si>
-  <si>
-    <t>Locatie</t>
-  </si>
-  <si>
     <t>person</t>
   </si>
   <si>
@@ -488,9 +461,6 @@
     <t>d_level2_id</t>
   </si>
   <si>
-    <t>Token.token</t>
-  </si>
-  <si>
     <t>#48D1CC</t>
   </si>
   <si>
@@ -527,18 +497,12 @@
     <t>#120C28</t>
   </si>
   <si>
-    <t>token</t>
-  </si>
-  <si>
     <t>Version_ID</t>
   </si>
   <si>
     <t>Version</t>
   </si>
   <si>
-    <t>Version.version</t>
-  </si>
-  <si>
     <t>v1</t>
   </si>
   <si>
@@ -726,13 +690,67 @@
   </si>
   <si>
     <t>#ff4a00</t>
+  </si>
+  <si>
+    <t>dss_tab</t>
+  </si>
+  <si>
+    <t>Token</t>
+  </si>
+  <si>
+    <t>Blockchain</t>
+  </si>
+  <si>
+    <t>Project</t>
+  </si>
+  <si>
+    <t>filecoin</t>
+  </si>
+  <si>
+    <t>frax</t>
+  </si>
+  <si>
+    <t>osmosis</t>
+  </si>
+  <si>
+    <t>rocketpool</t>
+  </si>
+  <si>
+    <t>dydx</t>
+  </si>
+  <si>
+    <t>#0090FF</t>
+  </si>
+  <si>
+    <t>#000000</t>
+  </si>
+  <si>
+    <t>#CBC3E3</t>
+  </si>
+  <si>
+    <t>#7600bc</t>
+  </si>
+  <si>
+    <t>#FFA500</t>
+  </si>
+  <si>
+    <t>reserverights</t>
+  </si>
+  <si>
+    <t>yellow</t>
+  </si>
+  <si>
+    <t>lightgreen</t>
+  </si>
+  <si>
+    <t>ens</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -745,6 +763,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF202124"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -767,10 +791,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -786,6 +811,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1085,10 +1114,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{811E847D-1D99-4D4E-BEB5-8ECC254EF9D7}">
-  <dimension ref="A1:Y21"/>
+  <dimension ref="A1:V21"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1108,108 +1137,98 @@
     <col min="13" max="13" width="13.3984375" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="15.3984375" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="15.3984375" customWidth="1"/>
-    <col min="16" max="18" width="14.86328125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="8.59765625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="6.73046875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="7.53125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="7.9296875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="3.9296875" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="6.59765625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="8.59765625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="6.73046875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="7.53125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="7.9296875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="3.9296875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="6.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" t="s">
         <v>14</v>
       </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
         <v>15</v>
       </c>
-      <c r="E1" t="s">
+      <c r="H1" t="s">
         <v>16</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
         <v>17</v>
       </c>
-      <c r="G1" t="s">
+      <c r="J1" t="s">
         <v>18</v>
       </c>
-      <c r="H1" t="s">
+      <c r="K1" t="s">
         <v>19</v>
       </c>
-      <c r="I1" t="s">
+      <c r="L1" t="s">
         <v>20</v>
       </c>
-      <c r="J1" t="s">
+      <c r="M1" t="s">
         <v>21</v>
       </c>
-      <c r="K1" t="s">
+      <c r="N1" t="s">
         <v>22</v>
       </c>
-      <c r="L1" t="s">
+      <c r="O1" t="s">
+        <v>203</v>
+      </c>
+      <c r="P1" t="s">
         <v>23</v>
       </c>
-      <c r="M1" t="s">
+      <c r="Q1" t="s">
         <v>24</v>
       </c>
-      <c r="N1" t="s">
+      <c r="R1" t="s">
         <v>25</v>
       </c>
-      <c r="O1" t="s">
-        <v>215</v>
-      </c>
-      <c r="P1" t="s">
+      <c r="S1" t="s">
         <v>26</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="T1" t="s">
         <v>27</v>
       </c>
-      <c r="R1" t="s">
+      <c r="U1" t="s">
         <v>28</v>
       </c>
-      <c r="S1" t="s">
+      <c r="V1" t="s">
         <v>29</v>
       </c>
-      <c r="T1" t="s">
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>30</v>
       </c>
-      <c r="U1" t="s">
+      <c r="C2" t="s">
         <v>31</v>
       </c>
-      <c r="V1" t="s">
+      <c r="D2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" t="s">
         <v>32</v>
-      </c>
-      <c r="W1" t="s">
-        <v>33</v>
-      </c>
-      <c r="X1" t="s">
-        <v>34</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.45">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E2" t="s">
-        <v>38</v>
       </c>
       <c r="F2">
         <v>1</v>
@@ -1227,7 +1246,7 @@
         <v>1</v>
       </c>
       <c r="K2" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="M2">
         <v>1</v>
@@ -1236,51 +1255,42 @@
         <v>1</v>
       </c>
       <c r="O2" t="s">
-        <v>216</v>
+        <v>204</v>
       </c>
       <c r="P2" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>41</v>
-      </c>
-      <c r="R2" t="s">
-        <v>42</v>
+        <v>34</v>
+      </c>
+      <c r="R2">
+        <v>1</v>
       </c>
       <c r="S2" t="s">
-        <v>43</v>
+        <v>35</v>
+      </c>
+      <c r="T2" t="s">
+        <v>36</v>
       </c>
       <c r="U2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V2" t="s">
-        <v>44</v>
-      </c>
-      <c r="W2" t="s">
-        <v>45</v>
-      </c>
-      <c r="X2">
-        <v>0</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.45">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="C3" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="D3" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="E3" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="F3">
         <v>3</v>
@@ -1298,7 +1308,7 @@
         <v>2</v>
       </c>
       <c r="K3" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="L3" s="1">
         <v>4.0000000000000002E-4</v>
@@ -1310,51 +1320,42 @@
         <v>1</v>
       </c>
       <c r="O3" t="s">
-        <v>216</v>
+        <v>204</v>
       </c>
       <c r="P3" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q3" t="s">
+        <v>34</v>
+      </c>
+      <c r="R3">
+        <v>2</v>
+      </c>
+      <c r="S3" t="s">
+        <v>35</v>
+      </c>
+      <c r="T3" t="s">
+        <v>36</v>
+      </c>
+      <c r="U3">
+        <v>0</v>
+      </c>
+      <c r="V3" t="s">
         <v>41</v>
       </c>
-      <c r="R3" t="s">
-        <v>42</v>
-      </c>
-      <c r="S3" t="s">
-        <v>43</v>
-      </c>
-      <c r="U3">
-        <v>2</v>
-      </c>
-      <c r="V3" t="s">
-        <v>44</v>
-      </c>
-      <c r="W3" t="s">
-        <v>45</v>
-      </c>
-      <c r="X3">
-        <v>0</v>
-      </c>
-      <c r="Y3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.45">
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="C4" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="D4" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="E4" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="F4">
         <v>3</v>
@@ -1372,7 +1373,7 @@
         <v>1</v>
       </c>
       <c r="K4" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="M4">
         <v>3</v>
@@ -1381,51 +1382,42 @@
         <v>1</v>
       </c>
       <c r="O4" t="s">
-        <v>216</v>
+        <v>204</v>
       </c>
       <c r="P4" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>41</v>
-      </c>
-      <c r="R4" t="s">
-        <v>42</v>
+        <v>45</v>
+      </c>
+      <c r="R4">
+        <v>3</v>
       </c>
       <c r="S4" t="s">
-        <v>54</v>
+        <v>46</v>
+      </c>
+      <c r="T4" t="s">
+        <v>47</v>
       </c>
       <c r="U4">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="V4" t="s">
-        <v>55</v>
-      </c>
-      <c r="W4" t="s">
-        <v>56</v>
-      </c>
-      <c r="X4">
-        <v>0</v>
-      </c>
-      <c r="Y4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.45">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="C5" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="D5" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="E5" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="F5">
         <v>4</v>
@@ -1443,7 +1435,7 @@
         <v>1</v>
       </c>
       <c r="K5" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="M5">
         <v>1</v>
@@ -1452,51 +1444,42 @@
         <v>1</v>
       </c>
       <c r="O5" t="s">
-        <v>216</v>
+        <v>204</v>
       </c>
       <c r="P5" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>41</v>
-      </c>
-      <c r="R5" t="s">
-        <v>42</v>
+        <v>50</v>
+      </c>
+      <c r="R5">
+        <v>4</v>
       </c>
       <c r="S5" t="s">
-        <v>59</v>
+        <v>51</v>
+      </c>
+      <c r="T5" t="s">
+        <v>36</v>
       </c>
       <c r="U5">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="V5" t="s">
-        <v>60</v>
-      </c>
-      <c r="W5" t="s">
-        <v>45</v>
-      </c>
-      <c r="X5">
-        <v>0</v>
-      </c>
-      <c r="Y5" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.45">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="C6" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="D6" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="E6" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="F6">
         <v>5</v>
@@ -1514,7 +1497,7 @@
         <v>1</v>
       </c>
       <c r="K6" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="M6">
         <v>1</v>
@@ -1523,51 +1506,42 @@
         <v>1</v>
       </c>
       <c r="O6" t="s">
-        <v>216</v>
+        <v>204</v>
       </c>
       <c r="P6" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>41</v>
-      </c>
-      <c r="R6" t="s">
-        <v>42</v>
+        <v>56</v>
+      </c>
+      <c r="R6">
+        <v>5</v>
       </c>
       <c r="S6" t="s">
-        <v>65</v>
+        <v>57</v>
+      </c>
+      <c r="T6" t="s">
+        <v>36</v>
       </c>
       <c r="U6">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="V6" t="s">
-        <v>66</v>
-      </c>
-      <c r="W6" t="s">
-        <v>45</v>
-      </c>
-      <c r="X6">
-        <v>0</v>
-      </c>
-      <c r="Y6" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.45">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="C7" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="D7" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="E7" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="F7">
         <v>6</v>
@@ -1585,7 +1559,7 @@
         <v>1</v>
       </c>
       <c r="K7" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="M7">
         <v>1</v>
@@ -1594,51 +1568,42 @@
         <v>1</v>
       </c>
       <c r="O7" t="s">
-        <v>216</v>
+        <v>204</v>
       </c>
       <c r="P7" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>41</v>
-      </c>
-      <c r="R7" t="s">
-        <v>42</v>
+        <v>61</v>
+      </c>
+      <c r="R7">
+        <v>6</v>
       </c>
       <c r="S7" t="s">
-        <v>70</v>
+        <v>57</v>
+      </c>
+      <c r="T7" t="s">
+        <v>36</v>
       </c>
       <c r="U7">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="V7" t="s">
-        <v>66</v>
-      </c>
-      <c r="W7" t="s">
-        <v>45</v>
-      </c>
-      <c r="X7">
-        <v>0</v>
-      </c>
-      <c r="Y7" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.45">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="C8" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="D8" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="E8" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="F8">
         <v>1</v>
@@ -1656,7 +1621,7 @@
         <v>2</v>
       </c>
       <c r="K8" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="M8">
         <v>1</v>
@@ -1665,51 +1630,42 @@
         <v>1</v>
       </c>
       <c r="O8" t="s">
-        <v>216</v>
+        <v>204</v>
       </c>
       <c r="P8" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>41</v>
-      </c>
-      <c r="R8" t="s">
-        <v>42</v>
+        <v>61</v>
+      </c>
+      <c r="R8">
+        <v>7</v>
       </c>
       <c r="S8" t="s">
-        <v>70</v>
+        <v>57</v>
+      </c>
+      <c r="T8" t="s">
+        <v>36</v>
       </c>
       <c r="U8">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="V8" t="s">
-        <v>66</v>
-      </c>
-      <c r="W8" t="s">
-        <v>45</v>
-      </c>
-      <c r="X8">
-        <v>0</v>
-      </c>
-      <c r="Y8" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.45">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="C9" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="D9" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="E9" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="F9">
         <v>8</v>
@@ -1727,7 +1683,7 @@
         <v>1</v>
       </c>
       <c r="K9" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="M9">
         <v>3</v>
@@ -1736,51 +1692,42 @@
         <v>1</v>
       </c>
       <c r="O9" t="s">
-        <v>216</v>
+        <v>204</v>
       </c>
       <c r="P9" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q9" t="s">
-        <v>41</v>
-      </c>
-      <c r="R9" t="s">
-        <v>42</v>
+        <v>61</v>
+      </c>
+      <c r="R9">
+        <v>8</v>
       </c>
       <c r="S9" t="s">
-        <v>70</v>
+        <v>57</v>
+      </c>
+      <c r="T9" t="s">
+        <v>36</v>
       </c>
       <c r="U9">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="V9" t="s">
-        <v>66</v>
-      </c>
-      <c r="W9" t="s">
-        <v>45</v>
-      </c>
-      <c r="X9">
-        <v>0</v>
-      </c>
-      <c r="Y9" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.45">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="C10" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="D10" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="E10" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="F10">
         <v>9</v>
@@ -1798,7 +1745,7 @@
         <v>1</v>
       </c>
       <c r="K10" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="M10">
         <v>3</v>
@@ -1807,51 +1754,42 @@
         <v>1</v>
       </c>
       <c r="O10" t="s">
-        <v>216</v>
+        <v>204</v>
       </c>
       <c r="P10" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q10" t="s">
-        <v>41</v>
-      </c>
-      <c r="R10" t="s">
-        <v>42</v>
+        <v>45</v>
+      </c>
+      <c r="R10">
+        <v>9</v>
       </c>
       <c r="S10" t="s">
-        <v>54</v>
+        <v>57</v>
+      </c>
+      <c r="T10" t="s">
+        <v>36</v>
       </c>
       <c r="U10">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="V10" t="s">
-        <v>66</v>
-      </c>
-      <c r="W10" t="s">
-        <v>45</v>
-      </c>
-      <c r="X10">
-        <v>0</v>
-      </c>
-      <c r="Y10" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.45">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C11" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="D11" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="E11" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="F11">
         <v>10</v>
@@ -1869,7 +1807,7 @@
         <v>1</v>
       </c>
       <c r="K11" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="M11">
         <v>1</v>
@@ -1878,51 +1816,42 @@
         <v>1</v>
       </c>
       <c r="O11" t="s">
-        <v>217</v>
+        <v>205</v>
       </c>
       <c r="P11" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q11" t="s">
-        <v>41</v>
-      </c>
-      <c r="R11" t="s">
-        <v>42</v>
+        <v>76</v>
+      </c>
+      <c r="R11">
+        <v>10</v>
       </c>
       <c r="S11" t="s">
-        <v>85</v>
+        <v>57</v>
+      </c>
+      <c r="T11" t="s">
+        <v>47</v>
       </c>
       <c r="U11">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="V11" t="s">
-        <v>66</v>
-      </c>
-      <c r="W11" t="s">
-        <v>56</v>
-      </c>
-      <c r="X11">
-        <v>1</v>
-      </c>
-      <c r="Y11" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.45">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="C12" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="D12" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="E12" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="F12">
         <v>11</v>
@@ -1940,7 +1869,7 @@
         <v>1</v>
       </c>
       <c r="K12" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="M12">
         <v>1</v>
@@ -1949,51 +1878,42 @@
         <v>1</v>
       </c>
       <c r="O12" t="s">
-        <v>216</v>
+        <v>204</v>
       </c>
       <c r="P12" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q12" t="s">
-        <v>41</v>
-      </c>
-      <c r="R12" t="s">
-        <v>42</v>
+        <v>81</v>
+      </c>
+      <c r="R12">
+        <v>11</v>
       </c>
       <c r="S12" t="s">
-        <v>90</v>
+        <v>57</v>
+      </c>
+      <c r="T12" t="s">
+        <v>47</v>
       </c>
       <c r="U12">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="V12" t="s">
-        <v>66</v>
-      </c>
-      <c r="W12" t="s">
-        <v>56</v>
-      </c>
-      <c r="X12">
-        <v>1</v>
-      </c>
-      <c r="Y12" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.45">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="C13" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="D13" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="E13" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="F13">
         <v>12</v>
@@ -2011,7 +1931,7 @@
         <v>1</v>
       </c>
       <c r="K13" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="M13">
         <v>1</v>
@@ -2020,51 +1940,42 @@
         <v>1</v>
       </c>
       <c r="O13" t="s">
-        <v>216</v>
+        <v>204</v>
       </c>
       <c r="P13" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q13" t="s">
-        <v>41</v>
-      </c>
-      <c r="R13" t="s">
-        <v>42</v>
+        <v>81</v>
+      </c>
+      <c r="R13">
+        <v>12</v>
       </c>
       <c r="S13" t="s">
-        <v>90</v>
+        <v>57</v>
+      </c>
+      <c r="T13" t="s">
+        <v>47</v>
       </c>
       <c r="U13">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="V13" t="s">
-        <v>66</v>
-      </c>
-      <c r="W13" t="s">
-        <v>56</v>
-      </c>
-      <c r="X13">
-        <v>1</v>
-      </c>
-      <c r="Y13" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.45">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="C14" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="D14" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="E14" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="F14">
         <v>13</v>
@@ -2082,7 +1993,7 @@
         <v>1</v>
       </c>
       <c r="K14" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="M14">
         <v>1</v>
@@ -2091,51 +2002,42 @@
         <v>1</v>
       </c>
       <c r="O14" t="s">
-        <v>216</v>
+        <v>204</v>
       </c>
       <c r="P14" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q14" t="s">
-        <v>41</v>
-      </c>
-      <c r="R14" t="s">
-        <v>42</v>
+        <v>88</v>
+      </c>
+      <c r="R14">
+        <v>13</v>
       </c>
       <c r="S14" t="s">
-        <v>97</v>
+        <v>57</v>
+      </c>
+      <c r="T14" t="s">
+        <v>47</v>
       </c>
       <c r="U14">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="V14" t="s">
-        <v>66</v>
-      </c>
-      <c r="W14" t="s">
-        <v>56</v>
-      </c>
-      <c r="X14">
-        <v>1</v>
-      </c>
-      <c r="Y14" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.45">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="C15" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="D15" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="E15" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="F15">
         <v>12</v>
@@ -2153,7 +2055,7 @@
         <v>2</v>
       </c>
       <c r="K15" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="M15">
         <v>1</v>
@@ -2162,51 +2064,42 @@
         <v>1</v>
       </c>
       <c r="O15" t="s">
-        <v>216</v>
+        <v>204</v>
       </c>
       <c r="P15" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q15" t="s">
+        <v>81</v>
+      </c>
+      <c r="R15">
+        <v>14</v>
+      </c>
+      <c r="S15" t="s">
+        <v>57</v>
+      </c>
+      <c r="T15" t="s">
+        <v>47</v>
+      </c>
+      <c r="U15">
+        <v>1</v>
+      </c>
+      <c r="V15" t="s">
         <v>41</v>
       </c>
-      <c r="R15" t="s">
-        <v>42</v>
-      </c>
-      <c r="S15" t="s">
-        <v>90</v>
-      </c>
-      <c r="U15">
-        <v>14</v>
-      </c>
-      <c r="V15" t="s">
-        <v>66</v>
-      </c>
-      <c r="W15" t="s">
-        <v>56</v>
-      </c>
-      <c r="X15">
-        <v>1</v>
-      </c>
-      <c r="Y15" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.45">
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="C16" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="D16" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="E16" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="F16">
         <v>15</v>
@@ -2224,7 +2117,7 @@
         <v>1</v>
       </c>
       <c r="K16" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="M16">
         <v>1</v>
@@ -2233,51 +2126,42 @@
         <v>1</v>
       </c>
       <c r="O16" t="s">
-        <v>216</v>
+        <v>204</v>
       </c>
       <c r="P16" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q16" t="s">
-        <v>41</v>
-      </c>
-      <c r="R16" t="s">
-        <v>42</v>
+        <v>88</v>
+      </c>
+      <c r="R16">
+        <v>15</v>
       </c>
       <c r="S16" t="s">
-        <v>97</v>
+        <v>57</v>
+      </c>
+      <c r="T16" t="s">
+        <v>47</v>
       </c>
       <c r="U16">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="V16" t="s">
-        <v>66</v>
-      </c>
-      <c r="W16" t="s">
-        <v>56</v>
-      </c>
-      <c r="X16">
-        <v>1</v>
-      </c>
-      <c r="Y16" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.45">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>213</v>
+        <v>201</v>
       </c>
       <c r="C17" t="s">
-        <v>214</v>
+        <v>202</v>
       </c>
       <c r="D17" t="s">
-        <v>214</v>
+        <v>202</v>
       </c>
       <c r="E17" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="F17">
         <v>12</v>
@@ -2295,7 +2179,7 @@
         <v>2</v>
       </c>
       <c r="K17" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="M17">
         <v>1</v>
@@ -2304,51 +2188,42 @@
         <v>1</v>
       </c>
       <c r="O17" t="s">
-        <v>216</v>
+        <v>204</v>
       </c>
       <c r="P17" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q17" t="s">
+        <v>81</v>
+      </c>
+      <c r="R17">
+        <v>16</v>
+      </c>
+      <c r="S17" t="s">
+        <v>57</v>
+      </c>
+      <c r="T17" t="s">
+        <v>47</v>
+      </c>
+      <c r="U17">
+        <v>0</v>
+      </c>
+      <c r="V17" t="s">
         <v>41</v>
       </c>
-      <c r="R17" t="s">
-        <v>42</v>
-      </c>
-      <c r="S17" t="s">
-        <v>90</v>
-      </c>
-      <c r="U17">
-        <v>16</v>
-      </c>
-      <c r="V17" t="s">
-        <v>66</v>
-      </c>
-      <c r="W17" t="s">
-        <v>56</v>
-      </c>
-      <c r="X17">
-        <v>0</v>
-      </c>
-      <c r="Y17" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.45">
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>218</v>
+        <v>206</v>
       </c>
       <c r="C18" t="s">
-        <v>221</v>
+        <v>209</v>
       </c>
       <c r="D18" t="s">
-        <v>221</v>
+        <v>209</v>
       </c>
       <c r="E18" t="s">
-        <v>223</v>
+        <v>211</v>
       </c>
       <c r="F18">
         <v>17</v>
@@ -2366,7 +2241,7 @@
         <v>1</v>
       </c>
       <c r="K18" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="M18">
         <v>1</v>
@@ -2375,45 +2250,36 @@
         <v>1</v>
       </c>
       <c r="O18" t="s">
-        <v>217</v>
+        <v>205</v>
       </c>
       <c r="P18" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q18" t="s">
+        <v>50</v>
+      </c>
+      <c r="R18">
+        <v>17</v>
+      </c>
+      <c r="U18">
+        <v>1</v>
+      </c>
+      <c r="V18" t="s">
         <v>41</v>
       </c>
-      <c r="R18" t="s">
-        <v>42</v>
-      </c>
-      <c r="S18" t="s">
-        <v>59</v>
-      </c>
-      <c r="U18">
-        <v>17</v>
-      </c>
-      <c r="X18">
-        <v>1</v>
-      </c>
-      <c r="Y18" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.45">
+    </row>
+    <row r="19" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C19" t="s">
-        <v>222</v>
+        <v>210</v>
       </c>
       <c r="D19" t="s">
-        <v>222</v>
+        <v>210</v>
       </c>
       <c r="E19" t="s">
-        <v>223</v>
+        <v>211</v>
       </c>
       <c r="F19">
         <v>18</v>
@@ -2431,7 +2297,7 @@
         <v>1</v>
       </c>
       <c r="K19" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="M19">
         <v>1</v>
@@ -2440,45 +2306,36 @@
         <v>1</v>
       </c>
       <c r="O19" t="s">
-        <v>217</v>
+        <v>205</v>
       </c>
       <c r="P19" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q19" t="s">
-        <v>41</v>
-      </c>
-      <c r="R19" t="s">
-        <v>42</v>
-      </c>
-      <c r="S19" t="s">
-        <v>59</v>
+        <v>50</v>
+      </c>
+      <c r="R19">
+        <v>18</v>
       </c>
       <c r="U19">
-        <v>18</v>
-      </c>
-      <c r="X19">
-        <v>1</v>
-      </c>
-      <c r="Y19" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.45">
+        <v>1</v>
+      </c>
+      <c r="V19" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>220</v>
+        <v>208</v>
       </c>
       <c r="C20" t="s">
-        <v>226</v>
+        <v>214</v>
       </c>
       <c r="D20" t="s">
-        <v>226</v>
+        <v>214</v>
       </c>
       <c r="E20" t="s">
-        <v>223</v>
+        <v>211</v>
       </c>
       <c r="F20">
         <v>19</v>
@@ -2496,7 +2353,7 @@
         <v>1</v>
       </c>
       <c r="K20" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="M20">
         <v>1</v>
@@ -2505,45 +2362,36 @@
         <v>1</v>
       </c>
       <c r="O20" t="s">
-        <v>216</v>
+        <v>204</v>
       </c>
       <c r="P20" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q20" t="s">
-        <v>41</v>
-      </c>
-      <c r="R20" t="s">
-        <v>42</v>
-      </c>
-      <c r="S20" t="s">
-        <v>59</v>
+        <v>50</v>
+      </c>
+      <c r="R20">
+        <v>19</v>
       </c>
       <c r="U20">
-        <v>19</v>
-      </c>
-      <c r="X20">
-        <v>1</v>
-      </c>
-      <c r="Y20" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.45">
+        <v>1</v>
+      </c>
+      <c r="V20" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>224</v>
+        <v>212</v>
       </c>
       <c r="C21" t="s">
-        <v>225</v>
+        <v>213</v>
       </c>
       <c r="D21" t="s">
-        <v>225</v>
+        <v>213</v>
       </c>
       <c r="E21" t="s">
-        <v>223</v>
+        <v>211</v>
       </c>
       <c r="F21">
         <v>18</v>
@@ -2561,7 +2409,7 @@
         <v>2</v>
       </c>
       <c r="K21" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="M21">
         <v>1</v>
@@ -2570,28 +2418,19 @@
         <v>1</v>
       </c>
       <c r="O21" t="s">
-        <v>217</v>
+        <v>205</v>
       </c>
       <c r="P21" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q21" t="s">
+        <v>50</v>
+      </c>
+      <c r="R21">
+        <v>20</v>
+      </c>
+      <c r="U21">
+        <v>1</v>
+      </c>
+      <c r="V21" t="s">
         <v>41</v>
-      </c>
-      <c r="R21" t="s">
-        <v>42</v>
-      </c>
-      <c r="S21" t="s">
-        <v>59</v>
-      </c>
-      <c r="U21">
-        <v>20</v>
-      </c>
-      <c r="X21">
-        <v>1</v>
-      </c>
-      <c r="Y21" t="s">
-        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -2602,24 +2441,25 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9010067A-CF14-4F37-9F88-BA65B8775ED4}">
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="7.9296875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.9296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.59765625" customWidth="1"/>
-    <col min="5" max="5" width="10.46484375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.3984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.46484375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.9296875" customWidth="1"/>
+    <col min="4" max="4" width="19.265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.59765625" customWidth="1"/>
+    <col min="6" max="6" width="10.46484375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.3984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.46484375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2627,396 +2467,456 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>216</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>139</v>
-      </c>
       <c r="E1" t="s">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="F1" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+        <v>131</v>
+      </c>
+      <c r="G1" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>148</v>
+        <v>217</v>
       </c>
       <c r="D2" t="s">
-        <v>137</v>
+        <v>217</v>
       </c>
       <c r="E2" t="s">
-        <v>4</v>
+        <v>128</v>
       </c>
       <c r="F2" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+        <v>3</v>
+      </c>
+      <c r="G2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>3</v>
+        <v>218</v>
       </c>
       <c r="D3" t="s">
-        <v>135</v>
+        <v>218</v>
       </c>
       <c r="E3" t="s">
-        <v>6</v>
+        <v>126</v>
       </c>
       <c r="F3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+        <v>4</v>
+      </c>
+      <c r="G3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>5</v>
+        <v>219</v>
       </c>
       <c r="D4" t="s">
+        <v>219</v>
+      </c>
+      <c r="E4" t="s">
+        <v>129</v>
+      </c>
+      <c r="F4" t="s">
         <v>138</v>
       </c>
-      <c r="E4" t="s">
-        <v>147</v>
-      </c>
-      <c r="F4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="C5" t="s">
+        <v>218</v>
+      </c>
+      <c r="D5" t="s">
+        <v>218</v>
+      </c>
+      <c r="E5" t="s">
+        <v>126</v>
+      </c>
+      <c r="F5" t="s">
         <v>3</v>
       </c>
-      <c r="D5" t="s">
-        <v>135</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="G5" t="s">
         <v>4</v>
       </c>
-      <c r="F5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="C6" t="s">
-        <v>5</v>
+        <v>219</v>
       </c>
       <c r="D6" t="s">
-        <v>138</v>
+        <v>219</v>
       </c>
       <c r="E6" t="s">
-        <v>6</v>
+        <v>129</v>
       </c>
       <c r="F6" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="C7" t="s">
-        <v>164</v>
+        <v>152</v>
       </c>
       <c r="D7" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
       <c r="E7" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="F7" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+        <v>138</v>
+      </c>
+      <c r="G7" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="C8" t="s">
+        <v>218</v>
+      </c>
+      <c r="D8" t="s">
+        <v>218</v>
+      </c>
+      <c r="E8" t="s">
+        <v>126</v>
+      </c>
+      <c r="F8" t="s">
         <v>3</v>
       </c>
-      <c r="D8" t="s">
-        <v>135</v>
-      </c>
-      <c r="E8" t="s">
+      <c r="G8" t="s">
         <v>4</v>
       </c>
-      <c r="F8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="C9" t="s">
-        <v>5</v>
+        <v>219</v>
       </c>
       <c r="D9" t="s">
-        <v>138</v>
+        <v>219</v>
       </c>
       <c r="E9" t="s">
-        <v>6</v>
+        <v>129</v>
       </c>
       <c r="F9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A10">
         <v>12</v>
       </c>
       <c r="B10" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="C10" t="s">
-        <v>164</v>
+        <v>152</v>
       </c>
       <c r="D10" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
       <c r="E10" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="F10" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+        <v>138</v>
+      </c>
+      <c r="G10" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A11">
         <v>13</v>
       </c>
       <c r="B11" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="C11" t="s">
+        <v>218</v>
+      </c>
+      <c r="D11" t="s">
+        <v>218</v>
+      </c>
+      <c r="E11" t="s">
+        <v>126</v>
+      </c>
+      <c r="F11" t="s">
         <v>3</v>
       </c>
-      <c r="D11" t="s">
-        <v>135</v>
-      </c>
-      <c r="E11" t="s">
+      <c r="G11" t="s">
         <v>4</v>
       </c>
-      <c r="F11" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A12">
         <v>13</v>
       </c>
       <c r="B12" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="C12" t="s">
-        <v>5</v>
+        <v>219</v>
       </c>
       <c r="D12" t="s">
-        <v>138</v>
+        <v>219</v>
       </c>
       <c r="E12" t="s">
-        <v>6</v>
+        <v>129</v>
       </c>
       <c r="F12" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G12" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A13">
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="C13" t="s">
-        <v>164</v>
+        <v>152</v>
       </c>
       <c r="D13" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
       <c r="E13" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="F13" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+        <v>138</v>
+      </c>
+      <c r="G13" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A14">
         <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="C14" t="s">
+        <v>218</v>
+      </c>
+      <c r="D14" t="s">
+        <v>218</v>
+      </c>
+      <c r="E14" t="s">
+        <v>126</v>
+      </c>
+      <c r="F14" t="s">
         <v>3</v>
       </c>
-      <c r="D14" t="s">
-        <v>135</v>
-      </c>
-      <c r="E14" t="s">
+      <c r="G14" t="s">
         <v>4</v>
       </c>
-      <c r="F14" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="C15" t="s">
-        <v>5</v>
+        <v>219</v>
       </c>
       <c r="D15" t="s">
-        <v>138</v>
+        <v>219</v>
       </c>
       <c r="E15" t="s">
-        <v>6</v>
+        <v>129</v>
       </c>
       <c r="F15" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G15" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="C16" t="s">
+        <v>218</v>
+      </c>
+      <c r="D16" t="s">
+        <v>218</v>
+      </c>
+      <c r="E16" t="s">
+        <v>126</v>
+      </c>
+      <c r="F16" t="s">
         <v>3</v>
       </c>
-      <c r="D16" t="s">
-        <v>135</v>
-      </c>
-      <c r="E16" t="s">
-        <v>4</v>
-      </c>
-      <c r="F16" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G16" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17">
         <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>218</v>
+        <v>206</v>
       </c>
       <c r="C17" t="s">
-        <v>5</v>
+        <v>219</v>
       </c>
       <c r="D17" t="s">
-        <v>138</v>
+        <v>219</v>
       </c>
       <c r="E17" t="s">
-        <v>4</v>
+        <v>129</v>
       </c>
       <c r="F17" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
+        <v>3</v>
+      </c>
+      <c r="G17" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18">
         <v>18</v>
       </c>
       <c r="B18" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C18" t="s">
-        <v>5</v>
+        <v>219</v>
       </c>
       <c r="D18" t="s">
-        <v>138</v>
+        <v>219</v>
       </c>
       <c r="E18" t="s">
-        <v>4</v>
+        <v>129</v>
       </c>
       <c r="F18" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
+        <v>3</v>
+      </c>
+      <c r="G18" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A19">
         <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>220</v>
+        <v>208</v>
       </c>
       <c r="C19" t="s">
-        <v>5</v>
+        <v>219</v>
       </c>
       <c r="D19" t="s">
-        <v>138</v>
+        <v>219</v>
       </c>
       <c r="E19" t="s">
-        <v>4</v>
+        <v>129</v>
       </c>
       <c r="F19" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
+        <v>3</v>
+      </c>
+      <c r="G19" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A20">
         <v>20</v>
       </c>
       <c r="B20" t="s">
-        <v>224</v>
+        <v>212</v>
       </c>
       <c r="C20" t="s">
-        <v>5</v>
+        <v>219</v>
       </c>
       <c r="D20" t="s">
-        <v>138</v>
+        <v>219</v>
       </c>
       <c r="E20" t="s">
-        <v>4</v>
+        <v>129</v>
       </c>
       <c r="F20" t="s">
-        <v>4</v>
+        <v>3</v>
+      </c>
+      <c r="G20" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -3029,7 +2929,7 @@
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F16" sqref="A16:F16"/>
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3044,22 +2944,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C1" t="s">
+        <v>133</v>
+      </c>
+      <c r="D1" t="s">
+        <v>134</v>
+      </c>
+      <c r="E1" t="s">
         <v>135</v>
       </c>
-      <c r="B1" t="s">
-        <v>141</v>
-      </c>
-      <c r="C1" t="s">
-        <v>142</v>
-      </c>
-      <c r="D1" t="s">
-        <v>143</v>
-      </c>
-      <c r="E1" t="s">
-        <v>144</v>
-      </c>
       <c r="F1" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.45">
@@ -3067,19 +2967,19 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>170</v>
+        <v>158</v>
       </c>
       <c r="C2" t="s">
-        <v>170</v>
+        <v>158</v>
       </c>
       <c r="D2" t="s">
-        <v>170</v>
+        <v>158</v>
       </c>
       <c r="E2" t="s">
-        <v>103</v>
+        <v>218</v>
       </c>
       <c r="F2" t="s">
-        <v>199</v>
+        <v>187</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.45">
@@ -3087,19 +2987,19 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>171</v>
+        <v>159</v>
       </c>
       <c r="C3" t="s">
-        <v>171</v>
+        <v>159</v>
       </c>
       <c r="D3" t="s">
-        <v>171</v>
+        <v>159</v>
       </c>
       <c r="E3" t="s">
-        <v>103</v>
+        <v>218</v>
       </c>
       <c r="F3" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.45">
@@ -3107,19 +3007,19 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="C4" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="D4" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="E4" t="s">
-        <v>103</v>
+        <v>218</v>
       </c>
       <c r="F4" t="s">
-        <v>149</v>
+        <v>139</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.45">
@@ -3127,19 +3027,19 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>172</v>
+        <v>160</v>
       </c>
       <c r="C5" t="s">
-        <v>172</v>
+        <v>160</v>
       </c>
       <c r="D5" t="s">
-        <v>172</v>
+        <v>160</v>
       </c>
       <c r="E5" t="s">
-        <v>103</v>
+        <v>218</v>
       </c>
       <c r="F5" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.45">
@@ -3147,19 +3047,19 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>173</v>
+        <v>161</v>
       </c>
       <c r="C6" t="s">
-        <v>173</v>
+        <v>161</v>
       </c>
       <c r="D6" t="s">
-        <v>173</v>
+        <v>161</v>
       </c>
       <c r="E6" t="s">
-        <v>103</v>
+        <v>218</v>
       </c>
       <c r="F6" t="s">
-        <v>151</v>
+        <v>141</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.45">
@@ -3167,19 +3067,19 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>174</v>
+        <v>162</v>
       </c>
       <c r="C7" t="s">
-        <v>174</v>
+        <v>162</v>
       </c>
       <c r="D7" t="s">
-        <v>174</v>
+        <v>162</v>
       </c>
       <c r="E7" t="s">
-        <v>103</v>
+        <v>218</v>
       </c>
       <c r="F7" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.45">
@@ -3187,19 +3087,19 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>175</v>
+        <v>163</v>
       </c>
       <c r="C8" t="s">
-        <v>175</v>
+        <v>163</v>
       </c>
       <c r="D8" t="s">
-        <v>175</v>
+        <v>163</v>
       </c>
       <c r="E8" t="s">
-        <v>103</v>
+        <v>218</v>
       </c>
       <c r="F8" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.45">
@@ -3207,19 +3107,19 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>176</v>
+        <v>164</v>
       </c>
       <c r="C9" t="s">
-        <v>176</v>
+        <v>164</v>
       </c>
       <c r="D9" t="s">
-        <v>176</v>
+        <v>164</v>
       </c>
       <c r="E9" t="s">
-        <v>103</v>
+        <v>218</v>
       </c>
       <c r="F9" t="s">
-        <v>154</v>
+        <v>144</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.45">
@@ -3227,19 +3127,19 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>177</v>
+        <v>165</v>
       </c>
       <c r="C10" t="s">
-        <v>177</v>
+        <v>165</v>
       </c>
       <c r="D10" t="s">
-        <v>177</v>
+        <v>165</v>
       </c>
       <c r="E10" t="s">
-        <v>103</v>
+        <v>218</v>
       </c>
       <c r="F10" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.45">
@@ -3247,19 +3147,19 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="C11" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="D11" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="E11" t="s">
-        <v>103</v>
+        <v>218</v>
       </c>
       <c r="F11" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.45">
@@ -3267,19 +3167,19 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>178</v>
+        <v>166</v>
       </c>
       <c r="C12" t="s">
-        <v>178</v>
+        <v>166</v>
       </c>
       <c r="D12" t="s">
-        <v>178</v>
+        <v>166</v>
       </c>
       <c r="E12" t="s">
-        <v>103</v>
+        <v>218</v>
       </c>
       <c r="F12" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.45">
@@ -3287,19 +3187,19 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="C13" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="D13" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="E13" t="s">
-        <v>103</v>
+        <v>218</v>
       </c>
       <c r="F13" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.45">
@@ -3307,19 +3207,19 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>179</v>
+        <v>167</v>
       </c>
       <c r="C14" t="s">
-        <v>179</v>
+        <v>167</v>
       </c>
       <c r="D14" t="s">
-        <v>179</v>
+        <v>167</v>
       </c>
       <c r="E14" t="s">
-        <v>103</v>
+        <v>218</v>
       </c>
       <c r="F14" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.45">
@@ -3327,19 +3227,19 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>196</v>
+        <v>184</v>
       </c>
       <c r="C15" t="s">
-        <v>196</v>
+        <v>184</v>
       </c>
       <c r="D15" t="s">
-        <v>196</v>
+        <v>184</v>
       </c>
       <c r="E15" t="s">
-        <v>103</v>
+        <v>218</v>
       </c>
       <c r="F15" t="s">
-        <v>198</v>
+        <v>186</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.45">
@@ -3347,19 +3247,19 @@
         <v>0</v>
       </c>
       <c r="B16" t="s">
-        <v>211</v>
+        <v>199</v>
       </c>
       <c r="C16" t="s">
-        <v>211</v>
+        <v>199</v>
       </c>
       <c r="D16" t="s">
-        <v>211</v>
+        <v>199</v>
       </c>
       <c r="E16" t="s">
-        <v>103</v>
+        <v>218</v>
       </c>
       <c r="F16" t="s">
-        <v>212</v>
+        <v>200</v>
       </c>
     </row>
     <row r="20" spans="3:3" x14ac:dyDescent="0.45">
@@ -3374,10 +3274,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8F231CF-1F8C-4057-B510-9BE4FB409CB9}">
-  <dimension ref="A1:F33"/>
+  <dimension ref="A1:F40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3390,22 +3290,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="B1" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="C1" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="D1" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="E1" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="F1" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.45">
@@ -3413,19 +3313,19 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E2" t="s">
-        <v>8</v>
+        <v>219</v>
       </c>
       <c r="F2" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.45">
@@ -3433,19 +3333,19 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E3" t="s">
-        <v>8</v>
+        <v>219</v>
       </c>
       <c r="F3" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.45">
@@ -3453,19 +3353,19 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>180</v>
+        <v>168</v>
       </c>
       <c r="C4" t="s">
-        <v>180</v>
+        <v>168</v>
       </c>
       <c r="D4" t="s">
-        <v>180</v>
+        <v>168</v>
       </c>
       <c r="E4" t="s">
-        <v>8</v>
+        <v>219</v>
       </c>
       <c r="F4" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.45">
@@ -3473,19 +3373,19 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>181</v>
+        <v>169</v>
       </c>
       <c r="C5" t="s">
-        <v>181</v>
+        <v>169</v>
       </c>
       <c r="D5" t="s">
-        <v>181</v>
+        <v>169</v>
       </c>
       <c r="E5" t="s">
-        <v>8</v>
+        <v>219</v>
       </c>
       <c r="F5" t="s">
-        <v>227</v>
+        <v>215</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.45">
@@ -3493,19 +3393,19 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
       <c r="C6" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
       <c r="D6" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
       <c r="E6" t="s">
-        <v>8</v>
+        <v>219</v>
       </c>
       <c r="F6" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.45">
@@ -3513,19 +3413,19 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="C7" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="D7" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="E7" t="s">
-        <v>8</v>
+        <v>219</v>
       </c>
       <c r="F7" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.45">
@@ -3533,19 +3433,19 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="C8" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="D8" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="E8" t="s">
-        <v>8</v>
+        <v>219</v>
       </c>
       <c r="F8" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.45">
@@ -3553,19 +3453,19 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="C9" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="D9" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="E9" t="s">
-        <v>8</v>
+        <v>219</v>
       </c>
       <c r="F9" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.45">
@@ -3573,19 +3473,19 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C10" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D10" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E10" t="s">
-        <v>8</v>
+        <v>219</v>
       </c>
       <c r="F10" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.45">
@@ -3593,19 +3493,19 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="C11" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="D11" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="E11" t="s">
-        <v>8</v>
+        <v>219</v>
       </c>
       <c r="F11" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.45">
@@ -3613,19 +3513,19 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="C12" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="D12" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="E12" t="s">
-        <v>8</v>
+        <v>219</v>
       </c>
       <c r="F12" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.45">
@@ -3633,19 +3533,19 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="C13" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="D13" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="E13" t="s">
-        <v>8</v>
+        <v>219</v>
       </c>
       <c r="F13" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.45">
@@ -3653,19 +3553,19 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>183</v>
+        <v>171</v>
       </c>
       <c r="C14" t="s">
-        <v>183</v>
+        <v>171</v>
       </c>
       <c r="D14" t="s">
-        <v>183</v>
+        <v>171</v>
       </c>
       <c r="E14" t="s">
-        <v>8</v>
+        <v>219</v>
       </c>
       <c r="F14" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.45">
@@ -3673,19 +3573,19 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>184</v>
+        <v>172</v>
       </c>
       <c r="C15" t="s">
-        <v>184</v>
+        <v>172</v>
       </c>
       <c r="D15" t="s">
-        <v>184</v>
+        <v>172</v>
       </c>
       <c r="E15" t="s">
-        <v>8</v>
+        <v>219</v>
       </c>
       <c r="F15" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.45">
@@ -3693,19 +3593,19 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>185</v>
+        <v>173</v>
       </c>
       <c r="C16" t="s">
-        <v>185</v>
+        <v>173</v>
       </c>
       <c r="D16" t="s">
-        <v>185</v>
+        <v>173</v>
       </c>
       <c r="E16" t="s">
-        <v>8</v>
+        <v>219</v>
       </c>
       <c r="F16" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.45">
@@ -3713,19 +3613,19 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>186</v>
+        <v>174</v>
       </c>
       <c r="C17" t="s">
-        <v>186</v>
+        <v>174</v>
       </c>
       <c r="D17" t="s">
-        <v>186</v>
+        <v>174</v>
       </c>
       <c r="E17" t="s">
-        <v>8</v>
+        <v>219</v>
       </c>
       <c r="F17" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.45">
@@ -3733,19 +3633,19 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>187</v>
+        <v>175</v>
       </c>
       <c r="C18" t="s">
-        <v>187</v>
+        <v>175</v>
       </c>
       <c r="D18" t="s">
-        <v>187</v>
+        <v>175</v>
       </c>
       <c r="E18" t="s">
-        <v>8</v>
+        <v>219</v>
       </c>
       <c r="F18" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.45">
@@ -3753,19 +3653,19 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>188</v>
+        <v>176</v>
       </c>
       <c r="C19" t="s">
-        <v>188</v>
+        <v>176</v>
       </c>
       <c r="D19" t="s">
-        <v>188</v>
+        <v>176</v>
       </c>
       <c r="E19" t="s">
-        <v>8</v>
+        <v>219</v>
       </c>
       <c r="F19" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.45">
@@ -3773,19 +3673,19 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>189</v>
+        <v>177</v>
       </c>
       <c r="C20" t="s">
-        <v>189</v>
+        <v>177</v>
       </c>
       <c r="D20" t="s">
-        <v>189</v>
+        <v>177</v>
       </c>
       <c r="E20" t="s">
-        <v>8</v>
+        <v>219</v>
       </c>
       <c r="F20" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.45">
@@ -3793,19 +3693,19 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>190</v>
+        <v>178</v>
       </c>
       <c r="C21" t="s">
-        <v>190</v>
+        <v>178</v>
       </c>
       <c r="D21" t="s">
-        <v>190</v>
+        <v>178</v>
       </c>
       <c r="E21" t="s">
-        <v>8</v>
+        <v>219</v>
       </c>
       <c r="F21" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.45">
@@ -3813,19 +3713,19 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>191</v>
+        <v>179</v>
       </c>
       <c r="C22" t="s">
-        <v>191</v>
+        <v>179</v>
       </c>
       <c r="D22" t="s">
-        <v>191</v>
+        <v>179</v>
       </c>
       <c r="E22" t="s">
-        <v>8</v>
+        <v>219</v>
       </c>
       <c r="F22" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.45">
@@ -3833,19 +3733,19 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>192</v>
+        <v>180</v>
       </c>
       <c r="C23" t="s">
-        <v>192</v>
+        <v>180</v>
       </c>
       <c r="D23" t="s">
-        <v>192</v>
+        <v>180</v>
       </c>
       <c r="E23" t="s">
-        <v>8</v>
+        <v>219</v>
       </c>
       <c r="F23" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.45">
@@ -3853,19 +3753,19 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>193</v>
+        <v>181</v>
       </c>
       <c r="C24" t="s">
-        <v>193</v>
+        <v>181</v>
       </c>
       <c r="D24" t="s">
-        <v>193</v>
+        <v>181</v>
       </c>
       <c r="E24" t="s">
-        <v>8</v>
+        <v>219</v>
       </c>
       <c r="F24" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.45">
@@ -3873,19 +3773,19 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>194</v>
+        <v>182</v>
       </c>
       <c r="C25" t="s">
-        <v>194</v>
+        <v>182</v>
       </c>
       <c r="D25" t="s">
-        <v>194</v>
+        <v>182</v>
       </c>
       <c r="E25" t="s">
-        <v>8</v>
+        <v>219</v>
       </c>
       <c r="F25" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.45">
@@ -3893,19 +3793,19 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="C26" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="D26" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="E26" t="s">
-        <v>8</v>
+        <v>219</v>
       </c>
       <c r="F26" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.45">
@@ -3913,19 +3813,19 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="C27" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="D27" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="E27" t="s">
-        <v>8</v>
+        <v>219</v>
       </c>
       <c r="F27" t="s">
-        <v>208</v>
+        <v>196</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.45">
@@ -3933,19 +3833,19 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>201</v>
+        <v>189</v>
       </c>
       <c r="C28" t="s">
-        <v>201</v>
+        <v>189</v>
       </c>
       <c r="D28" t="s">
-        <v>201</v>
+        <v>189</v>
       </c>
       <c r="E28" t="s">
-        <v>8</v>
+        <v>219</v>
       </c>
       <c r="F28" t="s">
-        <v>210</v>
+        <v>198</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.45">
@@ -3953,19 +3853,19 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>200</v>
+        <v>188</v>
       </c>
       <c r="C29" t="s">
-        <v>200</v>
+        <v>188</v>
       </c>
       <c r="D29" t="s">
-        <v>200</v>
+        <v>188</v>
       </c>
       <c r="E29" t="s">
-        <v>8</v>
+        <v>219</v>
       </c>
       <c r="F29" t="s">
-        <v>209</v>
+        <v>197</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.45">
@@ -3973,19 +3873,19 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>202</v>
+        <v>190</v>
       </c>
       <c r="C30" t="s">
-        <v>202</v>
+        <v>190</v>
       </c>
       <c r="D30" t="s">
-        <v>202</v>
+        <v>190</v>
       </c>
       <c r="E30" t="s">
-        <v>8</v>
+        <v>219</v>
       </c>
       <c r="F30" t="s">
-        <v>207</v>
+        <v>195</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.45">
@@ -3993,19 +3893,19 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>203</v>
+        <v>191</v>
       </c>
       <c r="C31" t="s">
-        <v>203</v>
+        <v>191</v>
       </c>
       <c r="D31" t="s">
-        <v>203</v>
+        <v>191</v>
       </c>
       <c r="E31" t="s">
-        <v>8</v>
+        <v>219</v>
       </c>
       <c r="F31" t="s">
-        <v>206</v>
+        <v>194</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.45">
@@ -4013,39 +3913,179 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>204</v>
+        <v>192</v>
       </c>
       <c r="C32" t="s">
-        <v>204</v>
+        <v>192</v>
       </c>
       <c r="D32" t="s">
-        <v>204</v>
+        <v>192</v>
       </c>
       <c r="E32" t="s">
-        <v>8</v>
+        <v>219</v>
       </c>
       <c r="F32" t="s">
-        <v>205</v>
+        <v>193</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
+        <v>220</v>
+      </c>
+      <c r="C33" t="s">
+        <v>220</v>
+      </c>
+      <c r="D33" t="s">
+        <v>220</v>
+      </c>
+      <c r="E33" t="s">
+        <v>219</v>
+      </c>
+      <c r="F33" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
+        <v>221</v>
+      </c>
+      <c r="C34" t="s">
+        <v>221</v>
+      </c>
+      <c r="D34" t="s">
+        <v>221</v>
+      </c>
+      <c r="E34" t="s">
+        <v>219</v>
+      </c>
+      <c r="F34" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="15.4" x14ac:dyDescent="0.45">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
+        <v>222</v>
+      </c>
+      <c r="C35" t="s">
+        <v>222</v>
+      </c>
+      <c r="D35" t="s">
+        <v>222</v>
+      </c>
+      <c r="E35" t="s">
+        <v>219</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
+        <v>224</v>
+      </c>
+      <c r="C36" t="s">
+        <v>224</v>
+      </c>
+      <c r="D36" t="s">
+        <v>224</v>
+      </c>
+      <c r="E36" t="s">
+        <v>219</v>
+      </c>
+      <c r="F36" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37" t="s">
+        <v>223</v>
+      </c>
+      <c r="C37" t="s">
+        <v>223</v>
+      </c>
+      <c r="D37" t="s">
+        <v>223</v>
+      </c>
+      <c r="E37" t="s">
+        <v>219</v>
+      </c>
+      <c r="F37" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38" t="s">
+        <v>230</v>
+      </c>
+      <c r="C38" t="s">
+        <v>230</v>
+      </c>
+      <c r="D38" t="s">
+        <v>230</v>
+      </c>
+      <c r="E38" t="s">
+        <v>219</v>
+      </c>
+      <c r="F38" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39" t="s">
+        <v>233</v>
+      </c>
+      <c r="C39" t="s">
+        <v>233</v>
+      </c>
+      <c r="D39" t="s">
+        <v>233</v>
+      </c>
+      <c r="E39" t="s">
+        <v>219</v>
+      </c>
+      <c r="F39" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A40">
         <v>0</v>
       </c>
-      <c r="B33" t="s">
-        <v>211</v>
-      </c>
-      <c r="C33" t="s">
-        <v>211</v>
-      </c>
-      <c r="D33" t="s">
-        <v>211</v>
-      </c>
-      <c r="E33" t="s">
-        <v>103</v>
-      </c>
-      <c r="F33" t="s">
-        <v>212</v>
+      <c r="B40" t="s">
+        <v>199</v>
+      </c>
+      <c r="C40" t="s">
+        <v>199</v>
+      </c>
+      <c r="D40" t="s">
+        <v>199</v>
+      </c>
+      <c r="E40" t="s">
+        <v>219</v>
+      </c>
+      <c r="F40" t="s">
+        <v>200</v>
       </c>
     </row>
   </sheetData>
@@ -4060,7 +4100,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:F7"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -4070,22 +4110,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>162</v>
+        <v>151</v>
       </c>
       <c r="B1" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="C1" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="D1" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="E1" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="F1" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.45">
@@ -4093,19 +4133,19 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>165</v>
+        <v>153</v>
       </c>
       <c r="C2" t="s">
-        <v>165</v>
+        <v>153</v>
       </c>
       <c r="D2" t="s">
-        <v>165</v>
+        <v>153</v>
       </c>
       <c r="E2" t="s">
-        <v>163</v>
+        <v>152</v>
       </c>
       <c r="F2" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.45">
@@ -4113,19 +4153,19 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>166</v>
+        <v>154</v>
       </c>
       <c r="C3" t="s">
-        <v>166</v>
+        <v>154</v>
       </c>
       <c r="D3" t="s">
-        <v>166</v>
+        <v>154</v>
       </c>
       <c r="E3" t="s">
-        <v>163</v>
+        <v>152</v>
       </c>
       <c r="F3" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.45">
@@ -4133,19 +4173,19 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>167</v>
+        <v>155</v>
       </c>
       <c r="C4" t="s">
-        <v>167</v>
+        <v>155</v>
       </c>
       <c r="D4" t="s">
-        <v>167</v>
+        <v>155</v>
       </c>
       <c r="E4" t="s">
-        <v>163</v>
+        <v>152</v>
       </c>
       <c r="F4" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.45">
@@ -4153,19 +4193,19 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
       <c r="C5" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
       <c r="D5" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
       <c r="E5" t="s">
-        <v>163</v>
+        <v>152</v>
       </c>
       <c r="F5" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.45">
@@ -4173,19 +4213,19 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>169</v>
+        <v>157</v>
       </c>
       <c r="C6" t="s">
-        <v>169</v>
+        <v>157</v>
       </c>
       <c r="D6" t="s">
-        <v>169</v>
+        <v>157</v>
       </c>
       <c r="E6" t="s">
-        <v>163</v>
+        <v>152</v>
       </c>
       <c r="F6" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.45">
@@ -4193,19 +4233,19 @@
         <v>0</v>
       </c>
       <c r="B7" t="s">
-        <v>211</v>
+        <v>199</v>
       </c>
       <c r="C7" t="s">
-        <v>211</v>
+        <v>199</v>
       </c>
       <c r="D7" t="s">
-        <v>211</v>
+        <v>199</v>
       </c>
       <c r="E7" t="s">
-        <v>103</v>
+        <v>152</v>
       </c>
       <c r="F7" t="s">
-        <v>212</v>
+        <v>200</v>
       </c>
     </row>
   </sheetData>
@@ -4218,7 +4258,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:F5"/>
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -4228,22 +4268,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C1" t="s">
+        <v>133</v>
+      </c>
+      <c r="D1" t="s">
+        <v>134</v>
+      </c>
+      <c r="E1" t="s">
+        <v>135</v>
+      </c>
+      <c r="F1" t="s">
         <v>136</v>
-      </c>
-      <c r="B1" t="s">
-        <v>141</v>
-      </c>
-      <c r="C1" t="s">
-        <v>142</v>
-      </c>
-      <c r="D1" t="s">
-        <v>143</v>
-      </c>
-      <c r="E1" t="s">
-        <v>144</v>
-      </c>
-      <c r="F1" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.45">
@@ -4266,19 +4306,19 @@
         <v>0</v>
       </c>
       <c r="B5" t="s">
-        <v>211</v>
+        <v>199</v>
       </c>
       <c r="C5" t="s">
-        <v>211</v>
+        <v>199</v>
       </c>
       <c r="D5" t="s">
-        <v>211</v>
+        <v>199</v>
       </c>
       <c r="E5" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="F5" t="s">
-        <v>212</v>
+        <v>200</v>
       </c>
     </row>
   </sheetData>
@@ -4291,7 +4331,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -4305,22 +4345,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="B1" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="C1" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="D1" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="E1" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="F1" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.45">
@@ -4328,19 +4368,19 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E2" t="s">
-        <v>161</v>
+        <v>217</v>
       </c>
       <c r="F2" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.45">
@@ -4348,19 +4388,19 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E3" t="s">
-        <v>161</v>
+        <v>217</v>
       </c>
       <c r="F3" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.45">
@@ -4368,19 +4408,19 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D4" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E4" t="s">
-        <v>161</v>
+        <v>217</v>
       </c>
       <c r="F4" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.45">
@@ -4388,19 +4428,19 @@
         <v>0</v>
       </c>
       <c r="B5" t="s">
-        <v>211</v>
+        <v>199</v>
       </c>
       <c r="C5" t="s">
-        <v>211</v>
+        <v>199</v>
       </c>
       <c r="D5" t="s">
-        <v>211</v>
+        <v>199</v>
       </c>
       <c r="E5" t="s">
-        <v>103</v>
+        <v>217</v>
       </c>
       <c r="F5" t="s">
-        <v>212</v>
+        <v>200</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
polars added so improved performace
</commit_message>
<xml_diff>
--- a/src/assets/Attributes/dashboard_data/cookpi_per_pi.xlsx
+++ b/src/assets/Attributes/dashboard_data/cookpi_per_pi.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/635b278bdf232d4a/Documents/Projects/cookkpi/dashboard/src/assets/Attributes/dashboard_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="488" documentId="8_{47E6BB2F-6528-457D-B946-AC2DD46DA1AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{534007D4-6093-4491-BF81-26211A881C1C}"/>
+  <xr:revisionPtr revIDLastSave="495" documentId="8_{47E6BB2F-6528-457D-B946-AC2DD46DA1AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C7F7F7FF-9A5B-4D5B-AD5A-9764ABDC0C53}"/>
   <bookViews>
-    <workbookView xWindow="44880" yWindow="14940" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="6" xr2:uid="{C3CBD8BC-F3E4-49AF-9A7E-08CF129859BA}"/>
+    <workbookView xWindow="44880" yWindow="14940" windowWidth="29040" windowHeight="15720" xr2:uid="{C3CBD8BC-F3E4-49AF-9A7E-08CF129859BA}"/>
   </bookViews>
   <sheets>
     <sheet name="d_kpi" sheetId="8" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="770" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="699" uniqueCount="252">
   <si>
     <t>d_kpi_id</t>
   </si>
@@ -845,10 +845,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -1170,8 +1169,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{811E847D-1D99-4D4E-BEB5-8ECC254EF9D7}">
   <dimension ref="A1:V21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2980,23 +2979,22 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1946D3B-FB13-4362-A6A9-7749AC28F3D2}">
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="14.19921875" customWidth="1"/>
     <col min="2" max="2" width="11.1328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.86328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.59765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.86328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>126</v>
       </c>
@@ -3004,22 +3002,19 @@
         <v>132</v>
       </c>
       <c r="C1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="E1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="F1" t="s">
-        <v>136</v>
-      </c>
-      <c r="G1" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3030,19 +3025,16 @@
         <v>158</v>
       </c>
       <c r="D2" t="s">
-        <v>158</v>
+        <v>218</v>
       </c>
       <c r="E2" t="s">
-        <v>218</v>
+        <v>187</v>
       </c>
       <c r="F2" t="s">
-        <v>187</v>
-      </c>
-      <c r="G2" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>2</v>
       </c>
@@ -3053,19 +3045,16 @@
         <v>159</v>
       </c>
       <c r="D3" t="s">
-        <v>159</v>
+        <v>218</v>
       </c>
       <c r="E3" t="s">
-        <v>218</v>
+        <v>150</v>
       </c>
       <c r="F3" t="s">
-        <v>150</v>
-      </c>
-      <c r="G3" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>3</v>
       </c>
@@ -3076,19 +3065,16 @@
         <v>100</v>
       </c>
       <c r="D4" t="s">
-        <v>100</v>
+        <v>218</v>
       </c>
       <c r="E4" t="s">
-        <v>218</v>
+        <v>139</v>
       </c>
       <c r="F4" t="s">
-        <v>139</v>
-      </c>
-      <c r="G4" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>4</v>
       </c>
@@ -3099,19 +3085,16 @@
         <v>160</v>
       </c>
       <c r="D5" t="s">
-        <v>160</v>
+        <v>218</v>
       </c>
       <c r="E5" t="s">
-        <v>218</v>
+        <v>140</v>
       </c>
       <c r="F5" t="s">
-        <v>140</v>
-      </c>
-      <c r="G5" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>5</v>
       </c>
@@ -3122,19 +3105,16 @@
         <v>161</v>
       </c>
       <c r="D6" t="s">
-        <v>161</v>
+        <v>218</v>
       </c>
       <c r="E6" t="s">
-        <v>218</v>
+        <v>141</v>
       </c>
       <c r="F6" t="s">
-        <v>141</v>
-      </c>
-      <c r="G6" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>6</v>
       </c>
@@ -3145,19 +3125,16 @@
         <v>162</v>
       </c>
       <c r="D7" t="s">
-        <v>162</v>
+        <v>218</v>
       </c>
       <c r="E7" t="s">
-        <v>218</v>
+        <v>142</v>
       </c>
       <c r="F7" t="s">
-        <v>142</v>
-      </c>
-      <c r="G7" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>7</v>
       </c>
@@ -3168,19 +3145,16 @@
         <v>163</v>
       </c>
       <c r="D8" t="s">
-        <v>163</v>
+        <v>218</v>
       </c>
       <c r="E8" t="s">
-        <v>218</v>
+        <v>143</v>
       </c>
       <c r="F8" t="s">
-        <v>143</v>
-      </c>
-      <c r="G8" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>8</v>
       </c>
@@ -3191,19 +3165,16 @@
         <v>164</v>
       </c>
       <c r="D9" t="s">
-        <v>164</v>
+        <v>218</v>
       </c>
       <c r="E9" t="s">
-        <v>218</v>
+        <v>144</v>
       </c>
       <c r="F9" t="s">
-        <v>144</v>
-      </c>
-      <c r="G9" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10">
         <v>9</v>
       </c>
@@ -3214,19 +3185,16 @@
         <v>165</v>
       </c>
       <c r="D10" t="s">
-        <v>165</v>
+        <v>218</v>
       </c>
       <c r="E10" t="s">
-        <v>218</v>
+        <v>145</v>
       </c>
       <c r="F10" t="s">
-        <v>145</v>
-      </c>
-      <c r="G10" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11">
         <v>10</v>
       </c>
@@ -3237,19 +3205,16 @@
         <v>103</v>
       </c>
       <c r="D11" t="s">
-        <v>103</v>
+        <v>218</v>
       </c>
       <c r="E11" t="s">
-        <v>218</v>
+        <v>146</v>
       </c>
       <c r="F11" t="s">
-        <v>146</v>
-      </c>
-      <c r="G11" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A12">
         <v>11</v>
       </c>
@@ -3260,19 +3225,16 @@
         <v>166</v>
       </c>
       <c r="D12" t="s">
-        <v>166</v>
+        <v>218</v>
       </c>
       <c r="E12" t="s">
-        <v>218</v>
+        <v>147</v>
       </c>
       <c r="F12" t="s">
-        <v>147</v>
-      </c>
-      <c r="G12" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13">
         <v>12</v>
       </c>
@@ -3283,19 +3245,16 @@
         <v>101</v>
       </c>
       <c r="D13" t="s">
-        <v>101</v>
+        <v>218</v>
       </c>
       <c r="E13" t="s">
-        <v>218</v>
+        <v>148</v>
       </c>
       <c r="F13" t="s">
-        <v>148</v>
-      </c>
-      <c r="G13" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A14">
         <v>13</v>
       </c>
@@ -3306,19 +3265,16 @@
         <v>167</v>
       </c>
       <c r="D14" t="s">
-        <v>167</v>
+        <v>218</v>
       </c>
       <c r="E14" t="s">
-        <v>218</v>
+        <v>149</v>
       </c>
       <c r="F14" t="s">
-        <v>149</v>
-      </c>
-      <c r="G14" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A15">
         <v>14</v>
       </c>
@@ -3329,19 +3285,16 @@
         <v>184</v>
       </c>
       <c r="D15" t="s">
-        <v>184</v>
+        <v>218</v>
       </c>
       <c r="E15" t="s">
-        <v>218</v>
+        <v>186</v>
       </c>
       <c r="F15" t="s">
-        <v>186</v>
-      </c>
-      <c r="G15" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A16">
         <v>0</v>
       </c>
@@ -3352,17 +3305,11 @@
         <v>199</v>
       </c>
       <c r="D16" t="s">
-        <v>199</v>
+        <v>218</v>
       </c>
       <c r="E16" t="s">
-        <v>218</v>
-      </c>
-      <c r="F16" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="20" spans="3:3" x14ac:dyDescent="0.45">
-      <c r="C20" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -3373,22 +3320,22 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8F231CF-1F8C-4057-B510-9BE4FB409CB9}">
-  <dimension ref="A1:G48"/>
+  <dimension ref="A1:F48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="10.46484375" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="17.796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.86328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.59765625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.06640625" customWidth="1"/>
+    <col min="2" max="3" width="17.796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.86328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.59765625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.06640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>129</v>
       </c>
@@ -3396,22 +3343,19 @@
         <v>132</v>
       </c>
       <c r="C1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="E1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="F1" t="s">
-        <v>136</v>
-      </c>
-      <c r="G1" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>0</v>
       </c>
@@ -3422,16 +3366,13 @@
         <v>199</v>
       </c>
       <c r="D2" t="s">
-        <v>199</v>
+        <v>219</v>
       </c>
       <c r="E2" t="s">
-        <v>219</v>
-      </c>
-      <c r="F2" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>1</v>
       </c>
@@ -3442,19 +3383,16 @@
         <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>219</v>
       </c>
       <c r="E3" t="s">
-        <v>219</v>
+        <v>95</v>
       </c>
       <c r="F3" t="s">
-        <v>95</v>
-      </c>
-      <c r="G3" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>2</v>
       </c>
@@ -3465,19 +3403,16 @@
         <v>7</v>
       </c>
       <c r="D4" t="s">
-        <v>7</v>
+        <v>219</v>
       </c>
       <c r="E4" t="s">
-        <v>219</v>
+        <v>96</v>
       </c>
       <c r="F4" t="s">
-        <v>96</v>
-      </c>
-      <c r="G4" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>3</v>
       </c>
@@ -3488,16 +3423,13 @@
         <v>168</v>
       </c>
       <c r="D5" t="s">
-        <v>168</v>
+        <v>219</v>
       </c>
       <c r="E5" t="s">
-        <v>219</v>
-      </c>
-      <c r="F5" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>4</v>
       </c>
@@ -3508,19 +3440,16 @@
         <v>169</v>
       </c>
       <c r="D6" t="s">
-        <v>169</v>
+        <v>219</v>
       </c>
       <c r="E6" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="F6" t="s">
-        <v>215</v>
-      </c>
-      <c r="G6" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>5</v>
       </c>
@@ -3531,16 +3460,13 @@
         <v>170</v>
       </c>
       <c r="D7" t="s">
-        <v>170</v>
+        <v>219</v>
       </c>
       <c r="E7" t="s">
-        <v>219</v>
-      </c>
-      <c r="F7" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>6</v>
       </c>
@@ -3551,19 +3477,16 @@
         <v>100</v>
       </c>
       <c r="D8" t="s">
-        <v>100</v>
+        <v>219</v>
       </c>
       <c r="E8" t="s">
-        <v>219</v>
+        <v>99</v>
       </c>
       <c r="F8" t="s">
-        <v>99</v>
-      </c>
-      <c r="G8" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>7</v>
       </c>
@@ -3574,19 +3497,16 @@
         <v>101</v>
       </c>
       <c r="D9" t="s">
-        <v>101</v>
+        <v>219</v>
       </c>
       <c r="E9" t="s">
-        <v>219</v>
+        <v>102</v>
       </c>
       <c r="F9" t="s">
-        <v>102</v>
-      </c>
-      <c r="G9" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10">
         <v>8</v>
       </c>
@@ -3597,19 +3517,16 @@
         <v>103</v>
       </c>
       <c r="D10" t="s">
-        <v>103</v>
+        <v>219</v>
       </c>
       <c r="E10" t="s">
-        <v>219</v>
+        <v>104</v>
       </c>
       <c r="F10" t="s">
-        <v>104</v>
-      </c>
-      <c r="G10" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11">
         <v>9</v>
       </c>
@@ -3620,16 +3537,13 @@
         <v>6</v>
       </c>
       <c r="D11" t="s">
-        <v>6</v>
+        <v>219</v>
       </c>
       <c r="E11" t="s">
-        <v>219</v>
-      </c>
-      <c r="F11" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A12">
         <v>10</v>
       </c>
@@ -3640,19 +3554,16 @@
         <v>106</v>
       </c>
       <c r="D12" t="s">
-        <v>106</v>
+        <v>219</v>
       </c>
       <c r="E12" t="s">
-        <v>219</v>
+        <v>107</v>
       </c>
       <c r="F12" t="s">
-        <v>107</v>
-      </c>
-      <c r="G12" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13">
         <v>11</v>
       </c>
@@ -3663,19 +3574,16 @@
         <v>108</v>
       </c>
       <c r="D13" t="s">
-        <v>108</v>
+        <v>219</v>
       </c>
       <c r="E13" t="s">
-        <v>219</v>
+        <v>109</v>
       </c>
       <c r="F13" t="s">
-        <v>109</v>
-      </c>
-      <c r="G13" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A14">
         <v>12</v>
       </c>
@@ -3686,19 +3594,16 @@
         <v>110</v>
       </c>
       <c r="D14" t="s">
-        <v>110</v>
+        <v>219</v>
       </c>
       <c r="E14" t="s">
-        <v>219</v>
+        <v>111</v>
       </c>
       <c r="F14" t="s">
-        <v>111</v>
-      </c>
-      <c r="G14" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A15">
         <v>13</v>
       </c>
@@ -3709,16 +3614,13 @@
         <v>171</v>
       </c>
       <c r="D15" t="s">
-        <v>171</v>
+        <v>219</v>
       </c>
       <c r="E15" t="s">
-        <v>219</v>
-      </c>
-      <c r="F15" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A16">
         <v>14</v>
       </c>
@@ -3729,19 +3631,16 @@
         <v>172</v>
       </c>
       <c r="D16" t="s">
-        <v>172</v>
+        <v>219</v>
       </c>
       <c r="E16" t="s">
-        <v>219</v>
+        <v>113</v>
       </c>
       <c r="F16" t="s">
-        <v>113</v>
-      </c>
-      <c r="G16" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A17">
         <v>15</v>
       </c>
@@ -3752,16 +3651,13 @@
         <v>173</v>
       </c>
       <c r="D17" t="s">
-        <v>173</v>
+        <v>219</v>
       </c>
       <c r="E17" t="s">
-        <v>219</v>
-      </c>
-      <c r="F17" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A18">
         <v>16</v>
       </c>
@@ -3772,16 +3668,13 @@
         <v>174</v>
       </c>
       <c r="D18" t="s">
-        <v>174</v>
+        <v>219</v>
       </c>
       <c r="E18" t="s">
-        <v>219</v>
-      </c>
-      <c r="F18" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A19">
         <v>17</v>
       </c>
@@ -3792,16 +3685,13 @@
         <v>175</v>
       </c>
       <c r="D19" t="s">
-        <v>175</v>
+        <v>219</v>
       </c>
       <c r="E19" t="s">
-        <v>219</v>
-      </c>
-      <c r="F19" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A20">
         <v>18</v>
       </c>
@@ -3812,19 +3702,16 @@
         <v>176</v>
       </c>
       <c r="D20" t="s">
-        <v>176</v>
+        <v>219</v>
       </c>
       <c r="E20" t="s">
-        <v>219</v>
+        <v>117</v>
       </c>
       <c r="F20" t="s">
-        <v>117</v>
-      </c>
-      <c r="G20" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A21">
         <v>19</v>
       </c>
@@ -3835,16 +3722,13 @@
         <v>177</v>
       </c>
       <c r="D21" t="s">
-        <v>177</v>
+        <v>219</v>
       </c>
       <c r="E21" t="s">
-        <v>219</v>
-      </c>
-      <c r="F21" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A22">
         <v>20</v>
       </c>
@@ -3855,16 +3739,13 @@
         <v>178</v>
       </c>
       <c r="D22" t="s">
-        <v>178</v>
+        <v>219</v>
       </c>
       <c r="E22" t="s">
-        <v>219</v>
-      </c>
-      <c r="F22" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A23">
         <v>21</v>
       </c>
@@ -3875,16 +3756,13 @@
         <v>179</v>
       </c>
       <c r="D23" t="s">
-        <v>179</v>
+        <v>219</v>
       </c>
       <c r="E23" t="s">
-        <v>219</v>
-      </c>
-      <c r="F23" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A24">
         <v>22</v>
       </c>
@@ -3895,19 +3773,16 @@
         <v>180</v>
       </c>
       <c r="D24" t="s">
-        <v>180</v>
+        <v>219</v>
       </c>
       <c r="E24" t="s">
-        <v>219</v>
+        <v>121</v>
       </c>
       <c r="F24" t="s">
-        <v>121</v>
-      </c>
-      <c r="G24" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A25">
         <v>23</v>
       </c>
@@ -3918,16 +3793,13 @@
         <v>181</v>
       </c>
       <c r="D25" t="s">
-        <v>181</v>
+        <v>219</v>
       </c>
       <c r="E25" t="s">
-        <v>219</v>
-      </c>
-      <c r="F25" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A26">
         <v>24</v>
       </c>
@@ -3938,16 +3810,13 @@
         <v>182</v>
       </c>
       <c r="D26" t="s">
-        <v>182</v>
+        <v>219</v>
       </c>
       <c r="E26" t="s">
-        <v>219</v>
-      </c>
-      <c r="F26" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A27">
         <v>25</v>
       </c>
@@ -3958,16 +3827,13 @@
         <v>183</v>
       </c>
       <c r="D27" t="s">
-        <v>183</v>
+        <v>219</v>
       </c>
       <c r="E27" t="s">
-        <v>219</v>
-      </c>
-      <c r="F27" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A28">
         <v>26</v>
       </c>
@@ -3978,16 +3844,13 @@
         <v>125</v>
       </c>
       <c r="D28" t="s">
-        <v>125</v>
+        <v>219</v>
       </c>
       <c r="E28" t="s">
-        <v>219</v>
-      </c>
-      <c r="F28" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A29">
         <v>27</v>
       </c>
@@ -3998,16 +3861,13 @@
         <v>189</v>
       </c>
       <c r="D29" t="s">
-        <v>189</v>
+        <v>219</v>
       </c>
       <c r="E29" t="s">
-        <v>219</v>
-      </c>
-      <c r="F29" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A30">
         <v>28</v>
       </c>
@@ -4018,16 +3878,13 @@
         <v>188</v>
       </c>
       <c r="D30" t="s">
-        <v>188</v>
+        <v>219</v>
       </c>
       <c r="E30" t="s">
-        <v>219</v>
-      </c>
-      <c r="F30" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A31">
         <v>29</v>
       </c>
@@ -4038,19 +3895,16 @@
         <v>190</v>
       </c>
       <c r="D31" t="s">
-        <v>190</v>
+        <v>219</v>
       </c>
       <c r="E31" t="s">
-        <v>219</v>
+        <v>195</v>
       </c>
       <c r="F31" t="s">
-        <v>195</v>
-      </c>
-      <c r="G31" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A32">
         <v>30</v>
       </c>
@@ -4061,19 +3915,16 @@
         <v>191</v>
       </c>
       <c r="D32" t="s">
-        <v>191</v>
+        <v>219</v>
       </c>
       <c r="E32" t="s">
-        <v>219</v>
+        <v>194</v>
       </c>
       <c r="F32" t="s">
-        <v>194</v>
-      </c>
-      <c r="G32" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A33">
         <v>31</v>
       </c>
@@ -4084,16 +3935,13 @@
         <v>192</v>
       </c>
       <c r="D33" t="s">
-        <v>192</v>
+        <v>219</v>
       </c>
       <c r="E33" t="s">
-        <v>219</v>
-      </c>
-      <c r="F33" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A34">
         <v>32</v>
       </c>
@@ -4104,16 +3952,13 @@
         <v>220</v>
       </c>
       <c r="D34" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E34" t="s">
-        <v>219</v>
-      </c>
-      <c r="F34" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A35">
         <v>33</v>
       </c>
@@ -4124,16 +3969,13 @@
         <v>221</v>
       </c>
       <c r="D35" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="E35" t="s">
-        <v>219</v>
-      </c>
-      <c r="F35" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="15.4" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:6" ht="15.4" x14ac:dyDescent="0.45">
       <c r="A36">
         <v>34</v>
       </c>
@@ -4144,19 +3986,16 @@
         <v>222</v>
       </c>
       <c r="D36" t="s">
-        <v>222</v>
-      </c>
-      <c r="E36" t="s">
-        <v>219</v>
-      </c>
-      <c r="F36" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="E36" s="2" t="s">
         <v>227</v>
       </c>
-      <c r="G36" t="s">
+      <c r="F36" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A37">
         <v>35</v>
       </c>
@@ -4167,16 +4006,13 @@
         <v>224</v>
       </c>
       <c r="D37" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="E37" t="s">
-        <v>219</v>
-      </c>
-      <c r="F37" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A38">
         <v>36</v>
       </c>
@@ -4187,16 +4023,13 @@
         <v>223</v>
       </c>
       <c r="D38" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="E38" t="s">
-        <v>219</v>
-      </c>
-      <c r="F38" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A39">
         <v>37</v>
       </c>
@@ -4207,16 +4040,13 @@
         <v>230</v>
       </c>
       <c r="D39" t="s">
-        <v>230</v>
+        <v>219</v>
       </c>
       <c r="E39" t="s">
-        <v>219</v>
-      </c>
-      <c r="F39" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A40">
         <v>38</v>
       </c>
@@ -4227,16 +4057,13 @@
         <v>233</v>
       </c>
       <c r="D40" t="s">
-        <v>233</v>
+        <v>219</v>
       </c>
       <c r="E40" t="s">
-        <v>219</v>
-      </c>
-      <c r="F40" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A41">
         <v>39</v>
       </c>
@@ -4247,19 +4074,16 @@
         <v>184</v>
       </c>
       <c r="D41" t="s">
-        <v>184</v>
+        <v>219</v>
       </c>
       <c r="E41" t="s">
-        <v>219</v>
+        <v>186</v>
       </c>
       <c r="F41" t="s">
-        <v>186</v>
-      </c>
-      <c r="G41" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A42">
         <v>40</v>
       </c>
@@ -4270,19 +4094,16 @@
         <v>159</v>
       </c>
       <c r="D42" t="s">
-        <v>159</v>
+        <v>219</v>
       </c>
       <c r="E42" t="s">
-        <v>219</v>
+        <v>150</v>
       </c>
       <c r="F42" t="s">
-        <v>150</v>
-      </c>
-      <c r="G42" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A43">
         <v>41</v>
       </c>
@@ -4293,19 +4114,16 @@
         <v>234</v>
       </c>
       <c r="D43" t="s">
-        <v>234</v>
+        <v>219</v>
       </c>
       <c r="E43" t="s">
-        <v>219</v>
+        <v>35</v>
       </c>
       <c r="F43" t="s">
-        <v>35</v>
-      </c>
-      <c r="G43" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A44">
         <v>42</v>
       </c>
@@ -4316,16 +4134,13 @@
         <v>235</v>
       </c>
       <c r="D44" t="s">
-        <v>235</v>
+        <v>219</v>
       </c>
       <c r="E44" t="s">
-        <v>219</v>
-      </c>
-      <c r="F44" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A45">
         <v>43</v>
       </c>
@@ -4336,16 +4151,13 @@
         <v>65</v>
       </c>
       <c r="D45" t="s">
-        <v>65</v>
+        <v>219</v>
       </c>
       <c r="E45" t="s">
-        <v>219</v>
-      </c>
-      <c r="F45" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A46">
         <v>44</v>
       </c>
@@ -4356,19 +4168,16 @@
         <v>236</v>
       </c>
       <c r="D46" t="s">
-        <v>236</v>
+        <v>219</v>
       </c>
       <c r="E46" t="s">
-        <v>219</v>
+        <v>241</v>
       </c>
       <c r="F46" t="s">
-        <v>241</v>
-      </c>
-      <c r="G46" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A47">
         <v>45</v>
       </c>
@@ -4379,19 +4188,16 @@
         <v>237</v>
       </c>
       <c r="D47" t="s">
-        <v>237</v>
+        <v>219</v>
       </c>
       <c r="E47" t="s">
-        <v>219</v>
+        <v>242</v>
       </c>
       <c r="F47" t="s">
-        <v>242</v>
-      </c>
-      <c r="G47" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A48">
         <v>46</v>
       </c>
@@ -4402,15 +4208,12 @@
         <v>238</v>
       </c>
       <c r="D48" t="s">
-        <v>238</v>
+        <v>219</v>
       </c>
       <c r="E48" t="s">
-        <v>219</v>
+        <v>243</v>
       </c>
       <c r="F48" t="s">
-        <v>243</v>
-      </c>
-      <c r="G48" t="s">
         <v>244</v>
       </c>
     </row>
@@ -4584,19 +4387,21 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CACC4D5-D335-41D8-8112-738352D6C6FA}">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="14.59765625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.19921875" customWidth="1"/>
+    <col min="2" max="2" width="10.19921875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.9296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.19921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>127</v>
       </c>
@@ -4604,37 +4409,34 @@
         <v>132</v>
       </c>
       <c r="C1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="E1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="F1" t="s">
-        <v>136</v>
-      </c>
-      <c r="G1" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>0</v>
       </c>
@@ -4645,12 +4447,9 @@
         <v>199</v>
       </c>
       <c r="D5" t="s">
-        <v>199</v>
+        <v>94</v>
       </c>
       <c r="E5" t="s">
-        <v>94</v>
-      </c>
-      <c r="F5" t="s">
         <v>200</v>
       </c>
     </row>
@@ -4661,22 +4460,21 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4088C235-30A9-4FB8-A45A-F9A41BC2AB26}">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="2" max="2" width="10.19921875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.73046875" customWidth="1"/>
-    <col min="4" max="4" width="14.86328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.9296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.86328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.9296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>128</v>
       </c>
@@ -4684,22 +4482,19 @@
         <v>132</v>
       </c>
       <c r="C1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="E1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="F1" t="s">
-        <v>136</v>
-      </c>
-      <c r="G1" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>1</v>
       </c>
@@ -4710,16 +4505,13 @@
         <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>9</v>
+        <v>217</v>
       </c>
       <c r="E2" t="s">
-        <v>217</v>
-      </c>
-      <c r="F2" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>2</v>
       </c>
@@ -4730,16 +4522,13 @@
         <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>10</v>
+        <v>217</v>
       </c>
       <c r="E3" t="s">
-        <v>217</v>
-      </c>
-      <c r="F3" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>3</v>
       </c>
@@ -4750,16 +4539,13 @@
         <v>7</v>
       </c>
       <c r="D4" t="s">
-        <v>7</v>
+        <v>217</v>
       </c>
       <c r="E4" t="s">
-        <v>217</v>
-      </c>
-      <c r="F4" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>0</v>
       </c>
@@ -4770,12 +4556,9 @@
         <v>199</v>
       </c>
       <c r="D5" t="s">
-        <v>199</v>
+        <v>217</v>
       </c>
       <c r="E5" t="s">
-        <v>217</v>
-      </c>
-      <c r="F5" t="s">
         <v>200</v>
       </c>
     </row>

</xml_diff>